<commit_message>
cas de charge pour Michele le chef (1ère partie)
</commit_message>
<xml_diff>
--- a/SU_Suspension/13_Cas_de_charges/Cas de charges Invictus.xlsx
+++ b/SU_Suspension/13_Cas_de_charges/Cas de charges Invictus.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Martin Kawczynski\Documents\EPSA\GIT\STUF-2020\SU_Suspension\13_Cas_de_charges\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{93648634-3012-4684-A98A-1BDBE1B121C4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0C8E69EB-B7CD-49F9-81AC-8D2A4BFAE9E0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="857" firstSheet="7" activeTab="13" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="857" firstSheet="3" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Presentation" sheetId="1" r:id="rId1"/>
@@ -1137,7 +1137,73 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="135">
+  <dxfs count="134">
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
     <dxf>
       <border diagonalUp="0" diagonalDown="0">
         <left style="thin">
@@ -1316,26 +1382,6 @@
         </right>
         <top/>
         <bottom/>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right/>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
         <vertical style="thin">
           <color indexed="64"/>
         </vertical>
@@ -2818,72 +2864,6 @@
           <color indexed="64"/>
         </left>
         <right/>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
         <top style="thin">
           <color indexed="64"/>
         </top>
@@ -3703,34 +3683,34 @@
   </dxfs>
   <tableStyles count="6" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
     <tableStyle name="BRAKING 2G-style" pivot="0" count="3" xr9:uid="{00000000-0011-0000-FFFF-FFFF00000000}">
-      <tableStyleElement type="headerRow" dxfId="134"/>
-      <tableStyleElement type="firstRowStripe" dxfId="133"/>
-      <tableStyleElement type="secondRowStripe" dxfId="132"/>
+      <tableStyleElement type="headerRow" dxfId="133"/>
+      <tableStyleElement type="firstRowStripe" dxfId="132"/>
+      <tableStyleElement type="secondRowStripe" dxfId="131"/>
     </tableStyle>
     <tableStyle name="Left Turn 1G + Freinage 1-style" pivot="0" count="3" xr9:uid="{00000000-0011-0000-FFFF-FFFF01000000}">
-      <tableStyleElement type="headerRow" dxfId="131"/>
-      <tableStyleElement type="firstRowStripe" dxfId="130"/>
-      <tableStyleElement type="secondRowStripe" dxfId="129"/>
+      <tableStyleElement type="headerRow" dxfId="130"/>
+      <tableStyleElement type="firstRowStripe" dxfId="129"/>
+      <tableStyleElement type="secondRowStripe" dxfId="128"/>
     </tableStyle>
     <tableStyle name="LEFT TURN 2G-style" pivot="0" count="3" xr9:uid="{00000000-0011-0000-FFFF-FFFF02000000}">
-      <tableStyleElement type="headerRow" dxfId="128"/>
-      <tableStyleElement type="firstRowStripe" dxfId="127"/>
-      <tableStyleElement type="secondRowStripe" dxfId="126"/>
+      <tableStyleElement type="headerRow" dxfId="127"/>
+      <tableStyleElement type="firstRowStripe" dxfId="126"/>
+      <tableStyleElement type="secondRowStripe" dxfId="125"/>
     </tableStyle>
     <tableStyle name="Bump 3G-style" pivot="0" count="3" xr9:uid="{00000000-0011-0000-FFFF-FFFF03000000}">
-      <tableStyleElement type="headerRow" dxfId="125"/>
-      <tableStyleElement type="firstRowStripe" dxfId="124"/>
-      <tableStyleElement type="secondRowStripe" dxfId="123"/>
+      <tableStyleElement type="headerRow" dxfId="124"/>
+      <tableStyleElement type="firstRowStripe" dxfId="123"/>
+      <tableStyleElement type="secondRowStripe" dxfId="122"/>
     </tableStyle>
     <tableStyle name="INVERSE BRAKING 0.5G-style" pivot="0" count="3" xr9:uid="{00000000-0011-0000-FFFF-FFFF04000000}">
-      <tableStyleElement type="headerRow" dxfId="122"/>
-      <tableStyleElement type="firstRowStripe" dxfId="121"/>
-      <tableStyleElement type="secondRowStripe" dxfId="120"/>
+      <tableStyleElement type="headerRow" dxfId="121"/>
+      <tableStyleElement type="firstRowStripe" dxfId="120"/>
+      <tableStyleElement type="secondRowStripe" dxfId="119"/>
     </tableStyle>
     <tableStyle name="Right Turn 1G + Freinage 1G-style" pivot="0" count="3" xr9:uid="{00000000-0011-0000-FFFF-FFFF05000000}">
-      <tableStyleElement type="headerRow" dxfId="119"/>
-      <tableStyleElement type="firstRowStripe" dxfId="118"/>
-      <tableStyleElement type="secondRowStripe" dxfId="117"/>
+      <tableStyleElement type="headerRow" dxfId="118"/>
+      <tableStyleElement type="firstRowStripe" dxfId="117"/>
+      <tableStyleElement type="secondRowStripe" dxfId="116"/>
     </tableStyle>
   </tableStyles>
   <extLst>
@@ -3850,15 +3830,15 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{C777FF87-0074-4175-8D63-A33A87A03168}" name="Table_229101134" displayName="Table_229101134" ref="D5:J49" headerRowDxfId="116" totalsRowDxfId="115">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{C777FF87-0074-4175-8D63-A33A87A03168}" name="Table_229101134" displayName="Table_229101134" ref="D5:J49" headerRowDxfId="115" totalsRowDxfId="114">
   <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{26D7065E-0723-49DD-942F-5EAB10B5F2C1}" name="Type" dataDxfId="114"/>
-    <tableColumn id="2" xr3:uid="{42E99A40-BE0F-4C4B-98ED-D788F5248E8E}" name="Part 1" dataDxfId="113"/>
-    <tableColumn id="3" xr3:uid="{846F5324-9AF6-4E17-AEDD-167092EBFE89}" name="Part 2" dataDxfId="112"/>
-    <tableColumn id="4" xr3:uid="{DBFCE167-4C49-4117-B3F5-5A68024F9A79}" name="Rx" dataDxfId="111"/>
-    <tableColumn id="5" xr3:uid="{F98C7914-8832-4F22-8145-EAA165B66FDF}" name="Ry" dataDxfId="110"/>
-    <tableColumn id="6" xr3:uid="{CDCF233B-4F79-4686-B71C-845D28EC7C60}" name="Rz" dataDxfId="109"/>
-    <tableColumn id="10" xr3:uid="{C86B6B54-B034-43FF-BA0B-855300888DE3}" name="F" dataDxfId="108">
+    <tableColumn id="1" xr3:uid="{26D7065E-0723-49DD-942F-5EAB10B5F2C1}" name="Type" dataDxfId="113"/>
+    <tableColumn id="2" xr3:uid="{42E99A40-BE0F-4C4B-98ED-D788F5248E8E}" name="Part 1" dataDxfId="112"/>
+    <tableColumn id="3" xr3:uid="{846F5324-9AF6-4E17-AEDD-167092EBFE89}" name="Part 2" dataDxfId="111"/>
+    <tableColumn id="4" xr3:uid="{DBFCE167-4C49-4117-B3F5-5A68024F9A79}" name="Rx" dataDxfId="110"/>
+    <tableColumn id="5" xr3:uid="{F98C7914-8832-4F22-8145-EAA165B66FDF}" name="Ry" dataDxfId="109"/>
+    <tableColumn id="6" xr3:uid="{CDCF233B-4F79-4686-B71C-845D28EC7C60}" name="Rz" dataDxfId="108"/>
+    <tableColumn id="10" xr3:uid="{C86B6B54-B034-43FF-BA0B-855300888DE3}" name="F" dataDxfId="107">
       <calculatedColumnFormula>SQRT(G6*G6+H6*H6+I6*I6)</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -3867,15 +3847,15 @@
 </file>
 
 <file path=xl/tables/table10.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{00000000-000C-0000-FFFF-FFFF04000000}" name="Table_226" displayName="Table_226" ref="D5:J50" headerRowDxfId="35" totalsRowDxfId="34">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{00000000-000C-0000-FFFF-FFFF04000000}" name="Table_226" displayName="Table_226" ref="D5:J50" headerRowDxfId="37" totalsRowDxfId="36">
   <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0400-000001000000}" name="Type" dataDxfId="33"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0400-000002000000}" name="Part 1" dataDxfId="32"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0400-000003000000}" name="Part 2" dataDxfId="31"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0400-000004000000}" name="Rx" dataDxfId="30"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0400-000005000000}" name="Ry" dataDxfId="29"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0400-000006000000}" name="Rz" dataDxfId="28"/>
-    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0400-00000A000000}" name="F" dataDxfId="27">
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0400-000001000000}" name="Type" dataDxfId="35"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0400-000002000000}" name="Part 1" dataDxfId="34"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0400-000003000000}" name="Part 2" dataDxfId="33"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0400-000004000000}" name="Rx" dataDxfId="32"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0400-000005000000}" name="Ry" dataDxfId="31"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0400-000006000000}" name="Rz" dataDxfId="30"/>
+    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0400-00000A000000}" name="F" dataDxfId="29">
       <calculatedColumnFormula>SQRT(G6*G6+H6*H6+I6*I6)</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -3884,15 +3864,15 @@
 </file>
 
 <file path=xl/tables/table11.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="9" xr:uid="{00000000-000C-0000-FFFF-FFFF05000000}" name="Table_22910" displayName="Table_22910" ref="D5:J48" headerRowDxfId="26" totalsRowDxfId="25">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="9" xr:uid="{00000000-000C-0000-FFFF-FFFF05000000}" name="Table_22910" displayName="Table_22910" ref="D5:J48" headerRowDxfId="28" totalsRowDxfId="27">
   <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0500-000001000000}" name="Type" dataDxfId="24"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0500-000002000000}" name="Part 1" dataDxfId="23"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0500-000003000000}" name="Part 2" dataDxfId="22"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0500-000004000000}" name="Rx" dataDxfId="21"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0500-000005000000}" name="Ry" dataDxfId="20"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0500-000006000000}" name="Rz" dataDxfId="19"/>
-    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0500-00000A000000}" name="F" dataDxfId="18">
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0500-000001000000}" name="Type" dataDxfId="26"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0500-000002000000}" name="Part 1" dataDxfId="25"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0500-000003000000}" name="Part 2" dataDxfId="24"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0500-000004000000}" name="Rx" dataDxfId="23"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0500-000005000000}" name="Ry" dataDxfId="22"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0500-000006000000}" name="Rz" dataDxfId="21"/>
+    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0500-00000A000000}" name="F" dataDxfId="20">
       <calculatedColumnFormula>SQRT(G6*G6+H6*H6+I6*I6)</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -3901,32 +3881,29 @@
 </file>
 
 <file path=xl/tables/table12.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="11" xr:uid="{00000000-000C-0000-FFFF-FFFF06000000}" name="Table_229101112" displayName="Table_229101112" ref="D5:J47" headerRowDxfId="17" totalsRowDxfId="16">
-  <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0600-000001000000}" name="Type" dataDxfId="15"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0600-000002000000}" name="Part 1" dataDxfId="14"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0600-000003000000}" name="Part 2" dataDxfId="13"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0600-000004000000}" name="Rx" dataDxfId="12"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0600-000005000000}" name="Ry" dataDxfId="11"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0600-000006000000}" name="Rz" dataDxfId="10"/>
-    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0600-00000A000000}" name="F" dataDxfId="9">
-      <calculatedColumnFormula>SQRT(G6*G6+H6*H6+I6*I6)</calculatedColumnFormula>
-    </tableColumn>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="11" xr:uid="{00000000-000C-0000-FFFF-FFFF06000000}" name="Table_229101112" displayName="Table_229101112" ref="D5:I50" headerRowDxfId="19" totalsRowDxfId="18">
+  <tableColumns count="6">
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0600-000001000000}" name="Type" dataDxfId="17"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0600-000002000000}" name="Part 1" dataDxfId="16"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0600-000003000000}" name="Part 2" dataDxfId="15"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0600-000004000000}" name="Rx" dataDxfId="14"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0600-000005000000}" name="Ry" dataDxfId="13"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0600-000006000000}" name="Rz" dataDxfId="12"/>
   </tableColumns>
   <tableStyleInfo name="BRAKING 2G-style" showFirstColumn="1" showLastColumn="1" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table13.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="12" xr:uid="{00000000-000C-0000-FFFF-FFFF07000000}" name="Table_22910111213" displayName="Table_22910111213" ref="D5:J47" headerRowDxfId="8" totalsRowDxfId="7">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="12" xr:uid="{00000000-000C-0000-FFFF-FFFF07000000}" name="Table_22910111213" displayName="Table_22910111213" ref="D5:J47" headerRowDxfId="11" totalsRowDxfId="10">
   <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0700-000001000000}" name="Type" dataDxfId="6"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0700-000002000000}" name="Part 1" dataDxfId="5"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0700-000003000000}" name="Part 2" dataDxfId="4"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0700-000004000000}" name="Rx" dataDxfId="3"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0700-000005000000}" name="Ry" dataDxfId="2"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0700-000006000000}" name="Rz" dataDxfId="1"/>
-    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0700-00000A000000}" name="F" dataDxfId="0">
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0700-000001000000}" name="Type" dataDxfId="9"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0700-000002000000}" name="Part 1" dataDxfId="8"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0700-000003000000}" name="Part 2" dataDxfId="7"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0700-000004000000}" name="Rx" dataDxfId="6"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0700-000005000000}" name="Ry" dataDxfId="5"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0700-000006000000}" name="Rz" dataDxfId="4"/>
+    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0700-00000A000000}" name="F" dataDxfId="3">
       <calculatedColumnFormula>SQRT(G6*G6+H6*H6+I6*I6)</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -3935,15 +3912,15 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table_22910113" displayName="Table_22910113" ref="D5:J49" headerRowDxfId="107" totalsRowDxfId="106">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table_22910113" displayName="Table_22910113" ref="D5:J49" headerRowDxfId="106" totalsRowDxfId="105">
   <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Type" dataDxfId="105"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Part 1" dataDxfId="104"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Part 2" dataDxfId="103"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Rx" dataDxfId="102"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="Ry" dataDxfId="101"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="Rz" dataDxfId="100"/>
-    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0000-00000A000000}" name="F" dataDxfId="99">
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Type" dataDxfId="104"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Part 1" dataDxfId="103"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Part 2" dataDxfId="102"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Rx" dataDxfId="101"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="Ry" dataDxfId="100"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="Rz" dataDxfId="99"/>
+    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0000-00000A000000}" name="F" dataDxfId="98">
       <calculatedColumnFormula>SQRT(G6*G6+H6*H6+I6*I6)</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -3952,15 +3929,15 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="10" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="Table_2291011" displayName="Table_2291011" ref="D5:J50" headerRowDxfId="98" totalsRowDxfId="97">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="10" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="Table_2291011" displayName="Table_2291011" ref="D5:J50" headerRowDxfId="97" totalsRowDxfId="96">
   <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0100-000001000000}" name="Type" dataDxfId="96"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0100-000002000000}" name="Part 1" dataDxfId="95"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0100-000003000000}" name="Part 2" dataDxfId="94"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0100-000004000000}" name="Rx" dataDxfId="93"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0100-000005000000}" name="Ry" dataDxfId="92"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0100-000006000000}" name="Rz" dataDxfId="91"/>
-    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0100-00000A000000}" name="F" dataDxfId="90">
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0100-000001000000}" name="Type" dataDxfId="95"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0100-000002000000}" name="Part 1" dataDxfId="94"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0100-000003000000}" name="Part 2" dataDxfId="93"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0100-000004000000}" name="Rx" dataDxfId="92"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0100-000005000000}" name="Ry" dataDxfId="91"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0100-000006000000}" name="Rz" dataDxfId="90"/>
+    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0100-00000A000000}" name="F" dataDxfId="89">
       <calculatedColumnFormula>SQRT(G6*G6+H6*H6+I6*I6)</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -3969,15 +3946,15 @@
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF02000000}" name="Table_22" displayName="Table_22" ref="D5:J47" headerRowDxfId="89" totalsRowDxfId="88">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF02000000}" name="Table_22" displayName="Table_22" ref="D5:J47" headerRowDxfId="88" totalsRowDxfId="87">
   <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0200-000001000000}" name="Type" dataDxfId="87"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0200-000002000000}" name="Part 1" dataDxfId="86"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0200-000003000000}" name="Part 2" dataDxfId="85"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0200-000004000000}" name="Rx" dataDxfId="84"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0200-000005000000}" name="Ry" dataDxfId="83"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0200-000006000000}" name="Rz" dataDxfId="82"/>
-    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0200-00000A000000}" name="F" dataDxfId="81">
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0200-000001000000}" name="Type" dataDxfId="86"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0200-000002000000}" name="Part 1" dataDxfId="85"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0200-000003000000}" name="Part 2" dataDxfId="84"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0200-000004000000}" name="Rx" dataDxfId="2"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0200-000005000000}" name="Ry" dataDxfId="1"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0200-000006000000}" name="Rz" dataDxfId="0"/>
+    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0200-00000A000000}" name="F" dataDxfId="83">
       <calculatedColumnFormula>SQRT(G6*G6+H6*H6+I6*I6)</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -3986,15 +3963,15 @@
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="13" xr:uid="{B0AFE184-AE6C-4FF3-8D63-F0BC8E23A6CF}" name="Table_2295814" displayName="Table_2295814" ref="D5:J50" headerRowDxfId="80" totalsRowDxfId="79">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="13" xr:uid="{B0AFE184-AE6C-4FF3-8D63-F0BC8E23A6CF}" name="Table_2295814" displayName="Table_2295814" ref="D5:J50" headerRowDxfId="82" totalsRowDxfId="81">
   <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{5CF42B42-17BB-4840-A98E-B5C21DA88B45}" name="Type" dataDxfId="78"/>
-    <tableColumn id="2" xr3:uid="{CA484149-8619-432A-AAEE-273B43A77EEB}" name="Part 1" dataDxfId="77"/>
-    <tableColumn id="3" xr3:uid="{153A0EC0-A7FA-4356-B034-40ABDE58108F}" name="Part 2" dataDxfId="76"/>
-    <tableColumn id="4" xr3:uid="{6438DE58-B6AF-4E59-A3B4-304BF0284DF3}" name="Rx" dataDxfId="75"/>
-    <tableColumn id="5" xr3:uid="{11464FEA-AD23-45DD-8207-9270CBF74988}" name="Ry" dataDxfId="74"/>
-    <tableColumn id="6" xr3:uid="{832F0331-1E22-477B-8D82-FCD2E083B4C0}" name="Rz" dataDxfId="73"/>
-    <tableColumn id="10" xr3:uid="{E2A35E5D-E1C6-41C4-A510-2FF34E76A089}" name="F" dataDxfId="72">
+    <tableColumn id="1" xr3:uid="{5CF42B42-17BB-4840-A98E-B5C21DA88B45}" name="Type" dataDxfId="80"/>
+    <tableColumn id="2" xr3:uid="{CA484149-8619-432A-AAEE-273B43A77EEB}" name="Part 1" dataDxfId="79"/>
+    <tableColumn id="3" xr3:uid="{153A0EC0-A7FA-4356-B034-40ABDE58108F}" name="Part 2" dataDxfId="78"/>
+    <tableColumn id="4" xr3:uid="{6438DE58-B6AF-4E59-A3B4-304BF0284DF3}" name="Rx" dataDxfId="77"/>
+    <tableColumn id="5" xr3:uid="{11464FEA-AD23-45DD-8207-9270CBF74988}" name="Ry" dataDxfId="76"/>
+    <tableColumn id="6" xr3:uid="{832F0331-1E22-477B-8D82-FCD2E083B4C0}" name="Rz" dataDxfId="75"/>
+    <tableColumn id="10" xr3:uid="{E2A35E5D-E1C6-41C4-A510-2FF34E76A089}" name="F" dataDxfId="74">
       <calculatedColumnFormula>SQRT(G6*G6+H6*H6+I6*I6)</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -4003,15 +3980,15 @@
 </file>
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{63497B11-6CFB-431E-8043-C5EA4856B019}" name="Table_22958" displayName="Table_22958" ref="D5:J50" headerRowDxfId="71" totalsRowDxfId="70">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{63497B11-6CFB-431E-8043-C5EA4856B019}" name="Table_22958" displayName="Table_22958" ref="D5:J50" headerRowDxfId="73" totalsRowDxfId="72">
   <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{C7C2A27F-B68F-4595-B3A6-80824AAEBE7E}" name="Type" dataDxfId="69"/>
-    <tableColumn id="2" xr3:uid="{F9164B72-0BB0-4A2B-AB4C-E9D021461BC3}" name="Part 1" dataDxfId="68"/>
-    <tableColumn id="3" xr3:uid="{E1FE5AA7-DF77-4186-B6D1-FCD4A338577B}" name="Part 2" dataDxfId="67"/>
-    <tableColumn id="4" xr3:uid="{E98E1800-10A5-4E7A-902F-83A63939A99C}" name="Rx" dataDxfId="66"/>
-    <tableColumn id="5" xr3:uid="{DF57FFDE-C9BB-4026-9267-B35746E5617B}" name="Ry" dataDxfId="65"/>
-    <tableColumn id="6" xr3:uid="{B76AC1C2-BF2D-435A-BC8A-DF791C33A631}" name="Rz" dataDxfId="64"/>
-    <tableColumn id="10" xr3:uid="{B94DD169-5874-4A11-82AB-41D75CE9E1C4}" name="F" dataDxfId="63">
+    <tableColumn id="1" xr3:uid="{C7C2A27F-B68F-4595-B3A6-80824AAEBE7E}" name="Type" dataDxfId="71"/>
+    <tableColumn id="2" xr3:uid="{F9164B72-0BB0-4A2B-AB4C-E9D021461BC3}" name="Part 1" dataDxfId="70"/>
+    <tableColumn id="3" xr3:uid="{E1FE5AA7-DF77-4186-B6D1-FCD4A338577B}" name="Part 2" dataDxfId="69"/>
+    <tableColumn id="4" xr3:uid="{E98E1800-10A5-4E7A-902F-83A63939A99C}" name="Rx" dataDxfId="68"/>
+    <tableColumn id="5" xr3:uid="{DF57FFDE-C9BB-4026-9267-B35746E5617B}" name="Ry" dataDxfId="67"/>
+    <tableColumn id="6" xr3:uid="{B76AC1C2-BF2D-435A-BC8A-DF791C33A631}" name="Rz" dataDxfId="66"/>
+    <tableColumn id="10" xr3:uid="{B94DD169-5874-4A11-82AB-41D75CE9E1C4}" name="F" dataDxfId="65">
       <calculatedColumnFormula>SQRT(G6*G6+H6*H6+I6*I6)</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -4020,15 +3997,15 @@
 </file>
 
 <file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{EEA5A4BA-6E68-456A-BA37-768ED05DFF03}" name="Table_2295" displayName="Table_2295" ref="D5:J50" headerRowDxfId="62" totalsRowDxfId="61">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{EEA5A4BA-6E68-456A-BA37-768ED05DFF03}" name="Table_2295" displayName="Table_2295" ref="D5:J50" headerRowDxfId="64" totalsRowDxfId="63">
   <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{0C6F79C5-B10E-4271-A5D4-4408A2063025}" name="Type" dataDxfId="60"/>
-    <tableColumn id="2" xr3:uid="{E86F6686-943D-4BC7-9D6F-FA4449FBAA83}" name="Part 1" dataDxfId="59"/>
-    <tableColumn id="3" xr3:uid="{2D13C6D0-4244-4392-980F-76660A4A5060}" name="Part 2" dataDxfId="58"/>
-    <tableColumn id="4" xr3:uid="{064AD1C3-3244-488D-BBFE-2B8CCB4B6B60}" name="Rx" dataDxfId="57"/>
-    <tableColumn id="5" xr3:uid="{7E162B99-B799-4078-9949-6F27B23EC330}" name="Ry" dataDxfId="56"/>
-    <tableColumn id="6" xr3:uid="{673CB13C-8584-493A-B7B1-E54129F7F8A7}" name="Rz" dataDxfId="55"/>
-    <tableColumn id="10" xr3:uid="{54734AB4-F9C8-4F27-8D94-075B17BBB2D5}" name="F" dataDxfId="54">
+    <tableColumn id="1" xr3:uid="{0C6F79C5-B10E-4271-A5D4-4408A2063025}" name="Type" dataDxfId="62"/>
+    <tableColumn id="2" xr3:uid="{E86F6686-943D-4BC7-9D6F-FA4449FBAA83}" name="Part 1" dataDxfId="61"/>
+    <tableColumn id="3" xr3:uid="{2D13C6D0-4244-4392-980F-76660A4A5060}" name="Part 2" dataDxfId="60"/>
+    <tableColumn id="4" xr3:uid="{064AD1C3-3244-488D-BBFE-2B8CCB4B6B60}" name="Rx" dataDxfId="59"/>
+    <tableColumn id="5" xr3:uid="{7E162B99-B799-4078-9949-6F27B23EC330}" name="Ry" dataDxfId="58"/>
+    <tableColumn id="6" xr3:uid="{673CB13C-8584-493A-B7B1-E54129F7F8A7}" name="Rz" dataDxfId="57"/>
+    <tableColumn id="10" xr3:uid="{54734AB4-F9C8-4F27-8D94-075B17BBB2D5}" name="F" dataDxfId="56">
       <calculatedColumnFormula>SQRT(G6*G6+H6*H6+I6*I6)</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -4037,15 +4014,15 @@
 </file>
 
 <file path=xl/tables/table8.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{D0C05053-3AE3-4D2D-9A69-48FE95801512}" name="Table_2297" displayName="Table_2297" ref="D2:J47" headerRowDxfId="53" totalsRowDxfId="52">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{D0C05053-3AE3-4D2D-9A69-48FE95801512}" name="Table_2297" displayName="Table_2297" ref="D2:J47" headerRowDxfId="55" totalsRowDxfId="54">
   <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{817511AE-EF59-4237-8AC4-BD3087668C1E}" name="Type" dataDxfId="51"/>
-    <tableColumn id="2" xr3:uid="{C5BA019C-B66B-499C-AB50-D0EE858D989B}" name="Part 1" dataDxfId="50"/>
-    <tableColumn id="3" xr3:uid="{734CB3FF-2256-439B-B403-9C5DE48737CB}" name="Part 2" dataDxfId="49"/>
-    <tableColumn id="4" xr3:uid="{E2A78AA9-3F71-4A43-8FD5-ABAEC128EA00}" name="Rx" dataDxfId="48"/>
-    <tableColumn id="5" xr3:uid="{2E02113B-8D48-42B2-ABCD-F2B6F3E2A60B}" name="Ry" dataDxfId="47"/>
-    <tableColumn id="6" xr3:uid="{055EC799-14EC-445A-A1B5-BEFABF90C4C5}" name="Rz" dataDxfId="46"/>
-    <tableColumn id="10" xr3:uid="{23D90AD4-2234-478E-9B30-A06F6533CDD2}" name="F" dataDxfId="45">
+    <tableColumn id="1" xr3:uid="{817511AE-EF59-4237-8AC4-BD3087668C1E}" name="Type" dataDxfId="53"/>
+    <tableColumn id="2" xr3:uid="{C5BA019C-B66B-499C-AB50-D0EE858D989B}" name="Part 1" dataDxfId="52"/>
+    <tableColumn id="3" xr3:uid="{734CB3FF-2256-439B-B403-9C5DE48737CB}" name="Part 2" dataDxfId="51"/>
+    <tableColumn id="4" xr3:uid="{E2A78AA9-3F71-4A43-8FD5-ABAEC128EA00}" name="Rx" dataDxfId="50"/>
+    <tableColumn id="5" xr3:uid="{2E02113B-8D48-42B2-ABCD-F2B6F3E2A60B}" name="Ry" dataDxfId="49"/>
+    <tableColumn id="6" xr3:uid="{055EC799-14EC-445A-A1B5-BEFABF90C4C5}" name="Rz" dataDxfId="48"/>
+    <tableColumn id="10" xr3:uid="{23D90AD4-2234-478E-9B30-A06F6533CDD2}" name="F" dataDxfId="47">
       <calculatedColumnFormula>SQRT(G3*G3+H3*H3+I3*I3)</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -4054,15 +4031,15 @@
 </file>
 
 <file path=xl/tables/table9.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{00000000-000C-0000-FFFF-FFFF03000000}" name="Table_229" displayName="Table_229" ref="D5:J50" headerRowDxfId="44" totalsRowDxfId="43">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{00000000-000C-0000-FFFF-FFFF03000000}" name="Table_229" displayName="Table_229" ref="D5:J50" headerRowDxfId="46" totalsRowDxfId="45">
   <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0300-000001000000}" name="Type" dataDxfId="42"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0300-000002000000}" name="Part 1" dataDxfId="41"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0300-000003000000}" name="Part 2" dataDxfId="40"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0300-000004000000}" name="Rx" dataDxfId="39"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0300-000005000000}" name="Ry" dataDxfId="38"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0300-000006000000}" name="Rz" dataDxfId="37"/>
-    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0300-00000A000000}" name="F" dataDxfId="36">
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0300-000001000000}" name="Type" dataDxfId="44"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0300-000002000000}" name="Part 1" dataDxfId="43"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0300-000003000000}" name="Part 2" dataDxfId="42"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0300-000004000000}" name="Rx" dataDxfId="41"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0300-000005000000}" name="Ry" dataDxfId="40"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0300-000006000000}" name="Rz" dataDxfId="39"/>
+    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0300-00000A000000}" name="F" dataDxfId="38">
       <calculatedColumnFormula>SQRT(G6*G6+H6*H6+I6*I6)</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -5617,8 +5594,8 @@
   </sheetPr>
   <dimension ref="A1:J1000"/>
   <sheetViews>
-    <sheetView topLeftCell="C16" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="O45" sqref="O45"/>
+    <sheetView topLeftCell="C13" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="L42" sqref="L42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -5715,17 +5692,17 @@
         <v>20</v>
       </c>
       <c r="G6" s="9">
-        <v>538.45699999999999</v>
+        <v>967.02</v>
       </c>
       <c r="H6" s="9">
-        <v>861.33900000000006</v>
+        <v>1235.9359999999999</v>
       </c>
       <c r="I6" s="9">
-        <v>275.154</v>
+        <v>508.637</v>
       </c>
       <c r="J6" s="16">
         <f t="shared" ref="J6:J47" si="0">SQRT(G6*G6+H6*H6+I6*I6)</f>
-        <v>1052.4022698027595</v>
+        <v>1649.659684378872</v>
       </c>
     </row>
     <row r="7" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -5746,17 +5723,17 @@
         <v>20</v>
       </c>
       <c r="G7" s="9">
-        <v>-538.53700000000003</v>
+        <v>-966.45299999999997</v>
       </c>
       <c r="H7" s="9">
-        <v>2584.1469999999999</v>
+        <v>1852.367</v>
       </c>
       <c r="I7" s="9">
-        <v>825.52499999999998</v>
+        <v>763.25599999999997</v>
       </c>
       <c r="J7" s="16">
         <f t="shared" si="0"/>
-        <v>2765.7420963645541</v>
+        <v>2224.3773567976277</v>
       </c>
     </row>
     <row r="8" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -5777,17 +5754,17 @@
         <v>20</v>
       </c>
       <c r="G8" s="9">
-        <v>419.28300000000002</v>
+        <v>709.39099999999996</v>
       </c>
       <c r="H8" s="9">
-        <v>-2795.2150000000001</v>
+        <v>-2216.8440000000001</v>
       </c>
       <c r="I8" s="9">
-        <v>-20.963999999999999</v>
+        <v>-17.734999999999999</v>
       </c>
       <c r="J8" s="16">
         <f t="shared" si="0"/>
-        <v>2826.5641014507351</v>
+        <v>2327.6484789250289</v>
       </c>
     </row>
     <row r="9" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -5808,17 +5785,17 @@
         <v>20</v>
       </c>
       <c r="G9" s="9">
-        <v>-419.33699999999999</v>
+        <v>-709.84299999999996</v>
       </c>
       <c r="H9" s="9">
-        <v>-931.86099999999999</v>
+        <v>-1478.8409999999999</v>
       </c>
       <c r="I9" s="9">
-        <v>-6.9889999999999999</v>
+        <v>-11.831</v>
       </c>
       <c r="J9" s="16">
         <f t="shared" si="0"/>
-        <v>1021.8890786239963</v>
+        <v>1640.4230431480166</v>
       </c>
     </row>
     <row r="10" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -5839,17 +5816,17 @@
         <v>35</v>
       </c>
       <c r="G10" s="9">
-        <v>538.45699999999999</v>
+        <v>967.02</v>
       </c>
       <c r="H10" s="9">
-        <v>861.32899999999995</v>
+        <v>1235.9259999999999</v>
       </c>
       <c r="I10" s="9">
-        <v>275.15199999999999</v>
+        <v>508.63400000000001</v>
       </c>
       <c r="J10" s="16">
         <f t="shared" si="0"/>
-        <v>1052.3935624061942</v>
+        <v>1649.6512673386455</v>
       </c>
     </row>
     <row r="11" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -5870,17 +5847,17 @@
         <v>38</v>
       </c>
       <c r="G11" s="9">
-        <v>-538.53700000000003</v>
+        <v>-966.45299999999997</v>
       </c>
       <c r="H11" s="9">
-        <v>2584.1469999999999</v>
+        <v>1852.367</v>
       </c>
       <c r="I11" s="9">
-        <v>825.52499999999998</v>
+        <v>763.25599999999997</v>
       </c>
       <c r="J11" s="16">
         <f t="shared" si="0"/>
-        <v>2765.7420963645541</v>
+        <v>2224.3773567976277</v>
       </c>
     </row>
     <row r="12" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -5901,17 +5878,17 @@
         <v>40</v>
       </c>
       <c r="G12" s="9">
-        <v>419.28300000000002</v>
+        <v>709.39099999999996</v>
       </c>
       <c r="H12" s="9">
-        <v>-2795.2150000000001</v>
+        <v>-2216.8440000000001</v>
       </c>
       <c r="I12" s="9">
-        <v>-20.963999999999999</v>
+        <v>-17.734999999999999</v>
       </c>
       <c r="J12" s="16">
         <f t="shared" si="0"/>
-        <v>2826.5641014507351</v>
+        <v>2327.6484789250289</v>
       </c>
     </row>
     <row r="13" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -5932,17 +5909,17 @@
         <v>42</v>
       </c>
       <c r="G13" s="9">
-        <v>-419.33699999999999</v>
+        <v>-709.84299999999996</v>
       </c>
       <c r="H13" s="9">
-        <v>-931.86099999999999</v>
+        <v>-1478.8409999999999</v>
       </c>
       <c r="I13" s="9">
-        <v>-6.9889999999999999</v>
+        <v>-11.831</v>
       </c>
       <c r="J13" s="16">
         <f t="shared" si="0"/>
-        <v>1021.8890786239963</v>
+        <v>1640.4230431480166</v>
       </c>
     </row>
     <row r="14" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -5963,17 +5940,17 @@
         <v>20</v>
       </c>
       <c r="G14" s="9">
-        <v>-0.01</v>
+        <v>-0.114</v>
       </c>
       <c r="H14" s="9">
-        <v>-6.5000000000000002E-2</v>
+        <v>-0.379</v>
       </c>
       <c r="I14" s="9">
-        <v>-6.0000000000000001E-3</v>
+        <v>-3.3000000000000002E-2</v>
       </c>
       <c r="J14" s="16">
         <f t="shared" si="0"/>
-        <v>6.6037867924396226E-2</v>
+        <v>0.39714732782684059</v>
       </c>
     </row>
     <row r="15" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -5994,17 +5971,17 @@
         <v>49</v>
       </c>
       <c r="G15" s="9">
-        <v>-0.01</v>
+        <v>-0.114</v>
       </c>
       <c r="H15" s="9">
-        <v>-6.5000000000000002E-2</v>
+        <v>-0.379</v>
       </c>
       <c r="I15" s="9">
-        <v>-6.0000000000000001E-3</v>
+        <v>-3.3000000000000002E-2</v>
       </c>
       <c r="J15" s="16">
         <f t="shared" si="0"/>
-        <v>6.6037867924396226E-2</v>
+        <v>0.39714732782684059</v>
       </c>
     </row>
     <row r="16" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -6025,17 +6002,17 @@
         <v>53</v>
       </c>
       <c r="G16" s="9">
-        <v>0.14399999999999999</v>
+        <v>0</v>
       </c>
       <c r="H16" s="9">
-        <v>-2345.3339999999998</v>
+        <v>-2019.2280000000001</v>
       </c>
       <c r="I16" s="9">
-        <v>803.70899999999995</v>
+        <v>634.13499999999999</v>
       </c>
       <c r="J16" s="16">
         <f t="shared" si="0"/>
-        <v>2479.2216014251326</v>
+        <v>2116.4614133522491</v>
       </c>
     </row>
     <row r="17" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -6056,17 +6033,17 @@
         <v>57</v>
       </c>
       <c r="G17" s="9">
-        <v>0.14399999999999999</v>
+        <v>0</v>
       </c>
       <c r="H17" s="9">
-        <v>-2345.3339999999998</v>
+        <v>-2019.2280000000001</v>
       </c>
       <c r="I17" s="9">
-        <v>803.70899999999995</v>
+        <v>634.13499999999999</v>
       </c>
       <c r="J17" s="16">
         <f t="shared" si="0"/>
-        <v>2479.2216014251326</v>
+        <v>2116.4614133522491</v>
       </c>
     </row>
     <row r="18" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -6090,14 +6067,14 @@
         <v>0</v>
       </c>
       <c r="H18" s="9">
-        <v>-1698.8030000000001</v>
+        <v>-1563.0930000000001</v>
       </c>
       <c r="I18" s="9">
-        <v>-453.96600000000001</v>
+        <v>-486.524</v>
       </c>
       <c r="J18" s="16">
         <f t="shared" si="0"/>
-        <v>1758.4131374523454</v>
+        <v>1637.059965066949</v>
       </c>
     </row>
     <row r="19" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -6121,14 +6098,14 @@
         <v>0</v>
       </c>
       <c r="H19" s="9">
-        <v>-1698.8030000000001</v>
+        <v>-1563.0930000000001</v>
       </c>
       <c r="I19" s="9">
-        <v>-453.96600000000001</v>
+        <v>-486.524</v>
       </c>
       <c r="J19" s="16">
         <f t="shared" si="0"/>
-        <v>1758.4131374523454</v>
+        <v>1637.059965066949</v>
       </c>
     </row>
     <row r="20" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -6149,17 +6126,17 @@
         <v>20</v>
       </c>
       <c r="G20" s="9">
-        <v>0.14399999999999999</v>
+        <v>0</v>
       </c>
       <c r="H20" s="9">
-        <v>-646.53</v>
+        <v>-456.13499999999999</v>
       </c>
       <c r="I20" s="9">
-        <v>1257.6759999999999</v>
+        <v>1120.6590000000001</v>
       </c>
       <c r="J20" s="16">
         <f t="shared" si="0"/>
-        <v>1414.1251651151676</v>
+        <v>1209.9321189661841</v>
       </c>
     </row>
     <row r="21" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -6217,11 +6194,11 @@
         <v>0</v>
       </c>
       <c r="I22" s="9">
-        <v>-1.45</v>
+        <v>-1.4530000000000001</v>
       </c>
       <c r="J22" s="16">
         <f t="shared" si="0"/>
-        <v>1.45</v>
+        <v>1.4530000000000001</v>
       </c>
     </row>
     <row r="23" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -6242,7 +6219,7 @@
         <v>78</v>
       </c>
       <c r="G23" s="9">
-        <v>-0.315</v>
+        <v>-0.314</v>
       </c>
       <c r="H23" s="9">
         <v>0</v>
@@ -6252,7 +6229,7 @@
       </c>
       <c r="J23" s="16">
         <f t="shared" si="0"/>
-        <v>7410.1450066952139</v>
+        <v>7410.1450066527714</v>
       </c>
     </row>
     <row r="24" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -6273,17 +6250,17 @@
         <v>78</v>
       </c>
       <c r="G24" s="9">
-        <v>0.315</v>
+        <v>0.314</v>
       </c>
       <c r="H24" s="9">
         <v>0</v>
       </c>
       <c r="I24" s="9">
-        <v>9288.0210000000006</v>
+        <v>9288.0239999999994</v>
       </c>
       <c r="J24" s="16">
         <f t="shared" si="0"/>
-        <v>9288.0210053415576</v>
+        <v>9288.0240053076941</v>
       </c>
     </row>
     <row r="25" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -6337,17 +6314,17 @@
         <v>20</v>
       </c>
       <c r="G26" s="9">
-        <v>-219.291</v>
+        <v>-165.02699999999999</v>
       </c>
       <c r="H26" s="9">
-        <v>-563.29</v>
+        <v>-390.91</v>
       </c>
       <c r="I26" s="9">
-        <v>30.291</v>
+        <v>21.658999999999999</v>
       </c>
       <c r="J26" s="16">
         <f t="shared" si="0"/>
-        <v>605.22864395367139</v>
+        <v>424.86898111064784</v>
       </c>
     </row>
     <row r="27" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -6368,17 +6345,17 @@
         <v>20</v>
       </c>
       <c r="G27" s="9">
-        <v>168.32</v>
+        <v>113.767</v>
       </c>
       <c r="H27" s="9">
-        <v>-432.084</v>
+        <v>-260.21499999999997</v>
       </c>
       <c r="I27" s="9">
-        <v>23.236000000000001</v>
+        <v>14.920999999999999</v>
       </c>
       <c r="J27" s="16">
         <f t="shared" si="0"/>
-        <v>464.29313709336691</v>
+        <v>284.38954403247664</v>
       </c>
     </row>
     <row r="28" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -6399,17 +6376,17 @@
         <v>20</v>
       </c>
       <c r="G28" s="9">
-        <v>607.81500000000005</v>
+        <v>589.31100000000004</v>
       </c>
       <c r="H28" s="9">
-        <v>-1575.76</v>
+        <v>-1527.789</v>
       </c>
       <c r="I28" s="9">
-        <v>174.155</v>
+        <v>168.85300000000001</v>
       </c>
       <c r="J28" s="16">
         <f t="shared" si="0"/>
-        <v>1697.8776798845081</v>
+        <v>1646.1889377744585</v>
       </c>
     </row>
     <row r="29" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -6430,17 +6407,17 @@
         <v>20</v>
       </c>
       <c r="G29" s="9">
-        <v>-562.32000000000005</v>
+        <v>-543.20299999999997</v>
       </c>
       <c r="H29" s="9">
-        <v>-1519.3409999999999</v>
+        <v>-1467.6890000000001</v>
       </c>
       <c r="I29" s="9">
-        <v>167.92</v>
+        <v>162.21100000000001</v>
       </c>
       <c r="J29" s="16">
         <f t="shared" si="0"/>
-        <v>1628.7412265553419</v>
+        <v>1573.3699210455879</v>
       </c>
     </row>
     <row r="30" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -6461,17 +6438,17 @@
         <v>99</v>
       </c>
       <c r="G30" s="9">
-        <v>-562.32000000000005</v>
+        <v>-543.20299999999997</v>
       </c>
       <c r="H30" s="9">
-        <v>-1519.3409999999999</v>
+        <v>-1467.6890000000001</v>
       </c>
       <c r="I30" s="9">
-        <v>167.92</v>
+        <v>162.21100000000001</v>
       </c>
       <c r="J30" s="16">
         <f t="shared" si="0"/>
-        <v>1628.7412265553419</v>
+        <v>1573.3699210455879</v>
       </c>
     </row>
     <row r="31" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -6492,17 +6469,17 @@
         <v>101</v>
       </c>
       <c r="G31" s="9">
-        <v>607.81500000000005</v>
+        <v>589.31100000000004</v>
       </c>
       <c r="H31" s="9">
-        <v>-1575.76</v>
+        <v>-1527.789</v>
       </c>
       <c r="I31" s="9">
-        <v>174.155</v>
+        <v>168.85300000000001</v>
       </c>
       <c r="J31" s="16">
         <f t="shared" si="0"/>
-        <v>1697.8776798845081</v>
+        <v>1646.1889377744585</v>
       </c>
     </row>
     <row r="32" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -6523,17 +6500,17 @@
         <v>103</v>
       </c>
       <c r="G32" s="9">
-        <v>168.32</v>
+        <v>113.767</v>
       </c>
       <c r="H32" s="9">
-        <v>-432.084</v>
+        <v>-260.21499999999997</v>
       </c>
       <c r="I32" s="9">
-        <v>23.236000000000001</v>
+        <v>14.920999999999999</v>
       </c>
       <c r="J32" s="16">
         <f t="shared" si="0"/>
-        <v>464.29313709336691</v>
+        <v>284.38954403247664</v>
       </c>
     </row>
     <row r="33" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -6554,17 +6531,17 @@
         <v>105</v>
       </c>
       <c r="G33" s="9">
-        <v>-219.291</v>
+        <v>-165.02699999999999</v>
       </c>
       <c r="H33" s="9">
-        <v>-563.29</v>
+        <v>-390.91</v>
       </c>
       <c r="I33" s="9">
-        <v>30.291</v>
+        <v>21.658999999999999</v>
       </c>
       <c r="J33" s="16">
         <f t="shared" si="0"/>
-        <v>605.22864395367139</v>
+        <v>424.86898111064784</v>
       </c>
     </row>
     <row r="34" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -6588,14 +6565,14 @@
         <v>0</v>
       </c>
       <c r="H34" s="9">
-        <v>1995.001</v>
+        <v>1519.768</v>
       </c>
       <c r="I34" s="9">
-        <v>1427.9739999999999</v>
+        <v>1459.05</v>
       </c>
       <c r="J34" s="16">
         <f t="shared" si="0"/>
-        <v>2453.3933102291203</v>
+        <v>2106.7799306818929</v>
       </c>
     </row>
     <row r="35" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -6619,14 +6596,14 @@
         <v>0</v>
       </c>
       <c r="H35" s="9">
-        <v>1995.001</v>
+        <v>1519.768</v>
       </c>
       <c r="I35" s="9">
-        <v>1427.9739999999999</v>
+        <v>1459.05</v>
       </c>
       <c r="J35" s="16">
         <f t="shared" si="0"/>
-        <v>2453.3933102291203</v>
+        <v>2106.7799306818929</v>
       </c>
     </row>
     <row r="36" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -6650,14 +6627,14 @@
         <v>0</v>
       </c>
       <c r="H36" s="9">
-        <v>-166.298</v>
+        <v>-222.488</v>
       </c>
       <c r="I36" s="9">
-        <v>1628.886</v>
+        <v>1771.5709999999999</v>
       </c>
       <c r="J36" s="16">
         <f t="shared" si="0"/>
-        <v>1637.3529325713498</v>
+        <v>1785.4872495162208</v>
       </c>
     </row>
     <row r="37" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -6681,14 +6658,14 @@
         <v>0</v>
       </c>
       <c r="H37" s="9">
-        <v>-166.298</v>
+        <v>-222.488</v>
       </c>
       <c r="I37" s="9">
-        <v>1628.886</v>
+        <v>1771.5709999999999</v>
       </c>
       <c r="J37" s="16">
         <f t="shared" si="0"/>
-        <v>1637.3529325713498</v>
+        <v>1785.4872495162208</v>
       </c>
     </row>
     <row r="38" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -6709,17 +6686,17 @@
         <v>119</v>
       </c>
       <c r="G38" s="9">
-        <v>5.476</v>
+        <v>5.1529999999999996</v>
       </c>
       <c r="H38" s="9">
-        <v>-531.52300000000002</v>
+        <v>-500.16300000000001</v>
       </c>
       <c r="I38" s="9">
-        <v>52.850999999999999</v>
+        <v>49.732999999999997</v>
       </c>
       <c r="J38" s="16">
         <f t="shared" si="0"/>
-        <v>534.17217664906514</v>
+        <v>502.65589747559909</v>
       </c>
     </row>
     <row r="39" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -6740,17 +6717,17 @@
         <v>20</v>
       </c>
       <c r="G39" s="9">
-        <v>5.476</v>
+        <v>5.1529999999999996</v>
       </c>
       <c r="H39" s="9">
-        <v>-531.52300000000002</v>
+        <v>-500.16300000000001</v>
       </c>
       <c r="I39" s="9">
-        <v>52.850999999999999</v>
+        <v>49.732999999999997</v>
       </c>
       <c r="J39" s="16">
         <f t="shared" si="0"/>
-        <v>534.17217664906514</v>
+        <v>502.65589747559909</v>
       </c>
     </row>
     <row r="40" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -6777,11 +6754,11 @@
         <v>0</v>
       </c>
       <c r="I40" s="9">
-        <v>221.98400000000001</v>
+        <v>221.983</v>
       </c>
       <c r="J40" s="16">
         <f t="shared" si="0"/>
-        <v>221.98400000000001</v>
+        <v>221.983</v>
       </c>
     </row>
     <row r="41" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -6867,14 +6844,14 @@
         <v>-1.238</v>
       </c>
       <c r="H43" s="9">
-        <v>-438.64699999999999</v>
+        <v>-438.64600000000002</v>
       </c>
       <c r="I43" s="9">
-        <v>9393.0910000000003</v>
+        <v>9393.0869999999995</v>
       </c>
       <c r="J43" s="16">
         <f t="shared" si="0"/>
-        <v>9403.3276693697117</v>
+        <v>9403.3236270761736</v>
       </c>
     </row>
     <row r="44" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -6901,11 +6878,11 @@
         <v>345.53100000000001</v>
       </c>
       <c r="I44" s="9">
-        <v>-7399.1329999999998</v>
+        <v>-7399.1289999999999</v>
       </c>
       <c r="J44" s="16">
         <f t="shared" si="0"/>
-        <v>7407.1966446413453</v>
+        <v>7407.1926489958396</v>
       </c>
     </row>
     <row r="45" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -6978,36 +6955,33 @@
       <c r="C47" s="13" t="s">
         <v>68</v>
       </c>
-      <c r="D47" s="43" t="s">
+      <c r="D47" s="9" t="s">
         <v>69</v>
       </c>
-      <c r="E47" s="43" t="s">
+      <c r="E47" s="9" t="s">
         <v>114</v>
       </c>
-      <c r="F47" s="43" t="s">
+      <c r="F47" s="9" t="s">
         <v>20</v>
       </c>
       <c r="G47" s="9">
         <v>0</v>
       </c>
       <c r="H47" s="9">
-        <v>2161.299</v>
+        <v>1742.2560000000001</v>
       </c>
       <c r="I47" s="9">
-        <v>-200.91399999999999</v>
-      </c>
-      <c r="J47" s="44">
-        <f t="shared" si="0"/>
-        <v>2170.6173782583146</v>
+        <v>-312.524</v>
+      </c>
+      <c r="J47" s="16">
+        <f t="shared" si="0"/>
+        <v>1770.0641853085442</v>
       </c>
     </row>
     <row r="48" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D48" s="36"/>
       <c r="E48" s="36"/>
       <c r="F48" s="36"/>
-      <c r="G48" s="36"/>
-      <c r="H48" s="36"/>
-      <c r="I48" s="36"/>
       <c r="J48" s="36"/>
     </row>
     <row r="49" spans="4:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -11830,8 +11804,8 @@
   </sheetPr>
   <dimension ref="A1:J1004"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="L29" sqref="L29"/>
+    <sheetView topLeftCell="A5" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="L28" sqref="L28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -11927,17 +11901,17 @@
         <v>20</v>
       </c>
       <c r="G6" s="9">
-        <v>417.09899999999999</v>
+        <v>749.07500000000005</v>
       </c>
       <c r="H6" s="9">
-        <v>667.14700000000005</v>
+        <v>957.31700000000001</v>
       </c>
       <c r="I6" s="9">
-        <v>213.125</v>
+        <v>393.98</v>
       </c>
       <c r="J6" s="16">
         <f t="shared" ref="J6:J47" si="0">SQRT(G6*G6+H6*H6+I6*I6)</f>
-        <v>815.15578942616855</v>
+        <v>1277.8064933760511</v>
       </c>
     </row>
     <row r="7" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -11958,17 +11932,17 @@
         <v>20</v>
       </c>
       <c r="G7" s="9">
-        <v>-417.161</v>
+        <v>-748.63599999999997</v>
       </c>
       <c r="H7" s="9">
-        <v>2001.732</v>
+        <v>1434.886</v>
       </c>
       <c r="I7" s="9">
-        <v>639.46799999999996</v>
+        <v>591.23599999999999</v>
       </c>
       <c r="J7" s="16">
         <f t="shared" si="0"/>
-        <v>2142.3990344398962</v>
+        <v>1723.0535978860321</v>
       </c>
     </row>
     <row r="8" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -11989,17 +11963,17 @@
         <v>20</v>
       </c>
       <c r="G8" s="9">
-        <v>324.779</v>
+        <v>549.49800000000005</v>
       </c>
       <c r="H8" s="9">
-        <v>-2165.19</v>
+        <v>-1717.182</v>
       </c>
       <c r="I8" s="9">
-        <v>-16.239000000000001</v>
+        <v>-13.737</v>
       </c>
       <c r="J8" s="16">
         <f t="shared" si="0"/>
-        <v>2189.4731877924428</v>
+        <v>1803.0115857356548</v>
       </c>
     </row>
     <row r="9" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -12020,17 +11994,17 @@
         <v>20</v>
       </c>
       <c r="G9" s="9">
-        <v>-324.82100000000003</v>
+        <v>-549.84900000000005</v>
       </c>
       <c r="H9" s="9">
-        <v>-721.82399999999996</v>
+        <v>-1145.519</v>
       </c>
       <c r="I9" s="9">
-        <v>-5.4139999999999997</v>
+        <v>-9.1639999999999997</v>
       </c>
       <c r="J9" s="16">
         <f t="shared" si="0"/>
-        <v>791.56040856841742</v>
+        <v>1270.6815813011535</v>
       </c>
     </row>
     <row r="10" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -12051,17 +12025,17 @@
         <v>35</v>
       </c>
       <c r="G10" s="9">
-        <v>417.09899999999999</v>
+        <v>749.07500000000005</v>
       </c>
       <c r="H10" s="9">
-        <v>667.14700000000005</v>
+        <v>957.31700000000001</v>
       </c>
       <c r="I10" s="9">
-        <v>213.125</v>
+        <v>393.98</v>
       </c>
       <c r="J10" s="16">
         <f t="shared" si="0"/>
-        <v>815.15578942616855</v>
+        <v>1277.8064933760511</v>
       </c>
     </row>
     <row r="11" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -12082,17 +12056,17 @@
         <v>38</v>
       </c>
       <c r="G11" s="9">
-        <v>-417.161</v>
+        <v>-748.63599999999997</v>
       </c>
       <c r="H11" s="9">
-        <v>2001.732</v>
+        <v>1434.886</v>
       </c>
       <c r="I11" s="9">
-        <v>639.46799999999996</v>
+        <v>591.23599999999999</v>
       </c>
       <c r="J11" s="16">
         <f t="shared" si="0"/>
-        <v>2142.3990344398962</v>
+        <v>1723.0535978860321</v>
       </c>
     </row>
     <row r="12" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -12113,17 +12087,17 @@
         <v>40</v>
       </c>
       <c r="G12" s="9">
-        <v>324.779</v>
+        <v>549.49800000000005</v>
       </c>
       <c r="H12" s="9">
-        <v>-2165.19</v>
+        <v>-1717.182</v>
       </c>
       <c r="I12" s="9">
-        <v>-16.239000000000001</v>
+        <v>-13.737</v>
       </c>
       <c r="J12" s="16">
         <f t="shared" si="0"/>
-        <v>2189.4731877924428</v>
+        <v>1803.0115857356548</v>
       </c>
     </row>
     <row r="13" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -12144,17 +12118,17 @@
         <v>42</v>
       </c>
       <c r="G13" s="9">
-        <v>-324.82100000000003</v>
+        <v>-549.84900000000005</v>
       </c>
       <c r="H13" s="9">
-        <v>-721.82399999999996</v>
+        <v>-1145.519</v>
       </c>
       <c r="I13" s="9">
-        <v>-5.4139999999999997</v>
+        <v>-9.1639999999999997</v>
       </c>
       <c r="J13" s="16">
         <f t="shared" si="0"/>
-        <v>791.56040856841742</v>
+        <v>1270.6815813011535</v>
       </c>
     </row>
     <row r="14" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -12175,17 +12149,17 @@
         <v>20</v>
       </c>
       <c r="G14" s="9">
-        <v>-8.0000000000000002E-3</v>
+        <v>-8.7999999999999995E-2</v>
       </c>
       <c r="H14" s="9">
-        <v>-5.0999999999999997E-2</v>
+        <v>-0.29199999999999998</v>
       </c>
       <c r="I14" s="9">
-        <v>-4.0000000000000001E-3</v>
+        <v>-2.5000000000000001E-2</v>
       </c>
       <c r="J14" s="16">
         <f t="shared" si="0"/>
-        <v>5.1778373863998466E-2</v>
+        <v>0.30599509799995162</v>
       </c>
     </row>
     <row r="15" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -12206,17 +12180,17 @@
         <v>49</v>
       </c>
       <c r="G15" s="9">
-        <v>-8.0000000000000002E-3</v>
+        <v>-8.7999999999999995E-2</v>
       </c>
       <c r="H15" s="9">
-        <v>-5.0999999999999997E-2</v>
+        <v>-0.29199999999999998</v>
       </c>
       <c r="I15" s="9">
-        <v>-4.0000000000000001E-3</v>
+        <v>-2.5000000000000001E-2</v>
       </c>
       <c r="J15" s="16">
         <f t="shared" si="0"/>
-        <v>5.1778373863998466E-2</v>
+        <v>0.30599509799995162</v>
       </c>
     </row>
     <row r="16" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -12237,17 +12211,17 @@
         <v>53</v>
       </c>
       <c r="G16" s="9">
-        <v>0.112</v>
+        <v>0</v>
       </c>
       <c r="H16" s="9">
-        <v>-1816.702</v>
+        <v>-1564.0989999999999</v>
       </c>
       <c r="I16" s="9">
-        <v>622.55499999999995</v>
+        <v>491.202</v>
       </c>
       <c r="J16" s="16">
         <f t="shared" si="0"/>
-        <v>1920.4116478955755</v>
+        <v>1639.4160809888988</v>
       </c>
     </row>
     <row r="17" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -12268,17 +12242,17 @@
         <v>57</v>
       </c>
       <c r="G17" s="9">
-        <v>0.112</v>
+        <v>0</v>
       </c>
       <c r="H17" s="9">
-        <v>-1816.702</v>
+        <v>-1564.0989999999999</v>
       </c>
       <c r="I17" s="9">
-        <v>622.55499999999995</v>
+        <v>491.202</v>
       </c>
       <c r="J17" s="16">
         <f t="shared" si="0"/>
-        <v>1920.4116478955755</v>
+        <v>1639.4160809888988</v>
       </c>
     </row>
     <row r="18" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -12302,14 +12276,14 @@
         <v>0</v>
       </c>
       <c r="H18" s="9">
-        <v>-1315.8979999999999</v>
+        <v>-1210.7750000000001</v>
       </c>
       <c r="I18" s="9">
-        <v>-351.64400000000001</v>
+        <v>-376.863</v>
       </c>
       <c r="J18" s="16">
         <f t="shared" si="0"/>
-        <v>1362.0723362362221</v>
+        <v>1268.0701169075787</v>
       </c>
     </row>
     <row r="19" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -12333,14 +12307,14 @@
         <v>0</v>
       </c>
       <c r="H19" s="9">
-        <v>-1315.8979999999999</v>
+        <v>-1210.7750000000001</v>
       </c>
       <c r="I19" s="9">
-        <v>-351.64400000000001</v>
+        <v>-376.863</v>
       </c>
       <c r="J19" s="16">
         <f t="shared" si="0"/>
-        <v>1362.0723362362221</v>
+        <v>1268.0701169075787</v>
       </c>
     </row>
     <row r="20" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -12361,17 +12335,17 @@
         <v>20</v>
       </c>
       <c r="G20" s="9">
-        <v>0.112</v>
+        <v>0</v>
       </c>
       <c r="H20" s="9">
-        <v>-500.803</v>
+        <v>-353.32299999999998</v>
       </c>
       <c r="I20" s="9">
-        <v>974.19899999999996</v>
+        <v>868.06500000000005</v>
       </c>
       <c r="J20" s="16">
         <f t="shared" si="0"/>
-        <v>1095.3845666951856</v>
+        <v>937.21608317079153</v>
       </c>
     </row>
     <row r="21" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -12398,11 +12372,11 @@
         <v>0</v>
       </c>
       <c r="I21" s="9">
-        <v>1453.492</v>
+        <v>1453.491</v>
       </c>
       <c r="J21" s="16">
         <f t="shared" si="0"/>
-        <v>1453.492</v>
+        <v>1453.491</v>
       </c>
     </row>
     <row r="22" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -12429,11 +12403,11 @@
         <v>0</v>
       </c>
       <c r="I22" s="9">
-        <v>-1.1200000000000001</v>
+        <v>-1.1220000000000001</v>
       </c>
       <c r="J22" s="16">
         <f t="shared" si="0"/>
-        <v>1.1200000000000001</v>
+        <v>1.1220000000000001</v>
       </c>
     </row>
     <row r="23" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -12454,7 +12428,7 @@
         <v>78</v>
       </c>
       <c r="G23" s="9">
-        <v>-0.245</v>
+        <v>-0.24099999999999999</v>
       </c>
       <c r="H23" s="9">
         <v>0</v>
@@ -12464,7 +12438,7 @@
       </c>
       <c r="J23" s="16">
         <f t="shared" si="0"/>
-        <v>5739.9460052287077</v>
+        <v>5739.946005059368</v>
       </c>
     </row>
     <row r="24" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -12485,17 +12459,17 @@
         <v>78</v>
       </c>
       <c r="G24" s="9">
-        <v>0.245</v>
+        <v>0.24099999999999999</v>
       </c>
       <c r="H24" s="9">
         <v>0</v>
       </c>
       <c r="I24" s="9">
-        <v>7194.558</v>
+        <v>7194.5590000000002</v>
       </c>
       <c r="J24" s="16">
         <f t="shared" si="0"/>
-        <v>7194.5580041715557</v>
+        <v>7194.5590040364532</v>
       </c>
     </row>
     <row r="25" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -12549,17 +12523,17 @@
         <v>20</v>
       </c>
       <c r="G26" s="9">
-        <v>-418.96800000000002</v>
+        <v>-355.988</v>
       </c>
       <c r="H26" s="9">
-        <v>-1076.1959999999999</v>
+        <v>-843.24900000000002</v>
       </c>
       <c r="I26" s="9">
-        <v>57.872999999999998</v>
+        <v>46.720999999999997</v>
       </c>
       <c r="J26" s="16">
         <f t="shared" si="0"/>
-        <v>1156.3223164710607</v>
+        <v>916.50378285416809</v>
       </c>
     </row>
     <row r="27" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -12580,17 +12554,17 @@
         <v>20</v>
       </c>
       <c r="G27" s="9">
-        <v>42.642000000000003</v>
+        <v>-22.666</v>
       </c>
       <c r="H27" s="9">
-        <v>-109.464</v>
+        <v>51.844000000000001</v>
       </c>
       <c r="I27" s="9">
-        <v>5.8860000000000001</v>
+        <v>-2.9729999999999999</v>
       </c>
       <c r="J27" s="16">
         <f t="shared" si="0"/>
-        <v>117.6237750456939</v>
+        <v>56.66027374625012</v>
       </c>
     </row>
     <row r="28" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -12611,17 +12585,17 @@
         <v>20</v>
       </c>
       <c r="G28" s="9">
-        <v>1201.838</v>
+        <v>1204.2429999999999</v>
       </c>
       <c r="H28" s="9">
-        <v>-3115.7649999999999</v>
+        <v>-3122</v>
       </c>
       <c r="I28" s="9">
-        <v>344.35899999999998</v>
+        <v>345.048</v>
       </c>
       <c r="J28" s="16">
         <f t="shared" si="0"/>
-        <v>3357.2293985293886</v>
+        <v>3363.9475806488126</v>
       </c>
     </row>
     <row r="29" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -12642,17 +12616,17 @@
         <v>20</v>
       </c>
       <c r="G29" s="9">
-        <v>-192.364</v>
+        <v>-190.511</v>
       </c>
       <c r="H29" s="9">
-        <v>-519.75199999999995</v>
+        <v>-514.745</v>
       </c>
       <c r="I29" s="9">
-        <v>57.444000000000003</v>
+        <v>56.89</v>
       </c>
       <c r="J29" s="16">
         <f t="shared" si="0"/>
-        <v>557.176689332926</v>
+        <v>551.80914114030406</v>
       </c>
     </row>
     <row r="30" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -12673,17 +12647,17 @@
         <v>99</v>
       </c>
       <c r="G30" s="9">
-        <v>-192.364</v>
+        <v>-190.511</v>
       </c>
       <c r="H30" s="9">
-        <v>-519.75199999999995</v>
+        <v>-514.745</v>
       </c>
       <c r="I30" s="9">
-        <v>57.444000000000003</v>
+        <v>56.89</v>
       </c>
       <c r="J30" s="16">
         <f t="shared" si="0"/>
-        <v>557.176689332926</v>
+        <v>551.80914114030406</v>
       </c>
     </row>
     <row r="31" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -12704,17 +12678,17 @@
         <v>101</v>
       </c>
       <c r="G31" s="9">
-        <v>1201.838</v>
+        <v>1204.2429999999999</v>
       </c>
       <c r="H31" s="9">
-        <v>-3115.7649999999999</v>
+        <v>-3122</v>
       </c>
       <c r="I31" s="9">
-        <v>344.35899999999998</v>
+        <v>345.048</v>
       </c>
       <c r="J31" s="16">
         <f t="shared" si="0"/>
-        <v>3357.2293985293886</v>
+        <v>3363.9475806488126</v>
       </c>
     </row>
     <row r="32" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -12735,17 +12709,17 @@
         <v>103</v>
       </c>
       <c r="G32" s="9">
-        <v>42.642000000000003</v>
+        <v>-22.666</v>
       </c>
       <c r="H32" s="9">
-        <v>-109.464</v>
+        <v>51.844000000000001</v>
       </c>
       <c r="I32" s="9">
-        <v>5.8860000000000001</v>
+        <v>-2.9729999999999999</v>
       </c>
       <c r="J32" s="16">
         <f t="shared" si="0"/>
-        <v>117.6237750456939</v>
+        <v>56.66027374625012</v>
       </c>
     </row>
     <row r="33" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -12766,17 +12740,17 @@
         <v>105</v>
       </c>
       <c r="G33" s="9">
-        <v>-418.96800000000002</v>
+        <v>-355.988</v>
       </c>
       <c r="H33" s="9">
-        <v>-1076.1959999999999</v>
+        <v>-843.24900000000002</v>
       </c>
       <c r="I33" s="9">
-        <v>57.872999999999998</v>
+        <v>46.720999999999997</v>
       </c>
       <c r="J33" s="16">
         <f t="shared" si="0"/>
-        <v>1156.3223164710607</v>
+        <v>916.50378285416809</v>
       </c>
     </row>
     <row r="34" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -12800,14 +12774,14 @@
         <v>0</v>
       </c>
       <c r="H34" s="9">
-        <v>2438.3679999999999</v>
+        <v>1858.058</v>
       </c>
       <c r="I34" s="9">
-        <v>1745.326</v>
+        <v>1783.8240000000001</v>
       </c>
       <c r="J34" s="16">
         <f t="shared" si="0"/>
-        <v>2998.6332469476824</v>
+        <v>2575.7343796168116</v>
       </c>
     </row>
     <row r="35" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -12831,14 +12805,14 @@
         <v>0</v>
       </c>
       <c r="H35" s="9">
-        <v>2438.3679999999999</v>
+        <v>1858.058</v>
       </c>
       <c r="I35" s="9">
-        <v>1745.326</v>
+        <v>1783.8240000000001</v>
       </c>
       <c r="J35" s="16">
         <f t="shared" si="0"/>
-        <v>2998.6332469476824</v>
+        <v>2575.7343796168116</v>
       </c>
     </row>
     <row r="36" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -12862,14 +12836,14 @@
         <v>0</v>
       </c>
       <c r="H36" s="9">
-        <v>-203.255</v>
+        <v>-272.01100000000002</v>
       </c>
       <c r="I36" s="9">
-        <v>1990.883</v>
+        <v>2165.902</v>
       </c>
       <c r="J36" s="16">
         <f t="shared" si="0"/>
-        <v>2001.2315494999575</v>
+        <v>2182.9158155377868</v>
       </c>
     </row>
     <row r="37" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -12893,14 +12867,14 @@
         <v>0</v>
       </c>
       <c r="H37" s="9">
-        <v>-203.255</v>
+        <v>-272.01100000000002</v>
       </c>
       <c r="I37" s="9">
-        <v>1990.883</v>
+        <v>2165.902</v>
       </c>
       <c r="J37" s="16">
         <f t="shared" si="0"/>
-        <v>2001.2315494999575</v>
+        <v>2182.9158155377868</v>
       </c>
     </row>
     <row r="38" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -12921,17 +12895,17 @@
         <v>119</v>
       </c>
       <c r="G38" s="9">
-        <v>8.5259999999999998</v>
+        <v>6.5970000000000004</v>
       </c>
       <c r="H38" s="9">
-        <v>-827.64800000000002</v>
+        <v>-640.36500000000001</v>
       </c>
       <c r="I38" s="9">
-        <v>82.296000000000006</v>
+        <v>63.673999999999999</v>
       </c>
       <c r="J38" s="16">
         <f t="shared" si="0"/>
-        <v>831.77312783955699</v>
+        <v>643.55670450240825</v>
       </c>
     </row>
     <row r="39" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -12952,17 +12926,17 @@
         <v>20</v>
       </c>
       <c r="G39" s="9">
-        <v>8.5259999999999998</v>
+        <v>6.5970000000000004</v>
       </c>
       <c r="H39" s="9">
-        <v>-827.64800000000002</v>
+        <v>-640.36500000000001</v>
       </c>
       <c r="I39" s="9">
-        <v>82.296000000000006</v>
+        <v>63.673999999999999</v>
       </c>
       <c r="J39" s="16">
         <f t="shared" si="0"/>
-        <v>831.77312783955699</v>
+        <v>643.55670450240825</v>
       </c>
     </row>
     <row r="40" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -13076,17 +13050,17 @@
         <v>126</v>
       </c>
       <c r="G43" s="9">
-        <v>110.639</v>
+        <v>110.64</v>
       </c>
       <c r="H43" s="9">
         <v>-511.85700000000003</v>
       </c>
       <c r="I43" s="9">
-        <v>10960.897000000001</v>
+        <v>10960.895</v>
       </c>
       <c r="J43" s="16">
         <f t="shared" si="0"/>
-        <v>10973.39972940834</v>
+        <v>10973.397741769593</v>
       </c>
     </row>
     <row r="44" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -13107,17 +13081,17 @@
         <v>126</v>
       </c>
       <c r="G44" s="9">
-        <v>530.91700000000003</v>
+        <v>530.91800000000001</v>
       </c>
       <c r="H44" s="9">
-        <v>470.05200000000002</v>
+        <v>470.05099999999999</v>
       </c>
       <c r="I44" s="9">
-        <v>-10065.168</v>
+        <v>-10065.166999999999</v>
       </c>
       <c r="J44" s="16">
         <f t="shared" si="0"/>
-        <v>10090.115391402469</v>
+        <v>10090.114399907168</v>
       </c>
     </row>
     <row r="45" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -13175,11 +13149,11 @@
         <v>0</v>
       </c>
       <c r="I46" s="9">
-        <v>1545.4269999999999</v>
+        <v>1545.4280000000001</v>
       </c>
       <c r="J46" s="16">
         <f t="shared" si="0"/>
-        <v>1545.4269999999999</v>
+        <v>1545.4280000000001</v>
       </c>
     </row>
     <row r="47" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -13203,33 +13177,48 @@
         <v>0</v>
       </c>
       <c r="H47" s="9">
-        <v>2641.623</v>
+        <v>2130.069</v>
       </c>
       <c r="I47" s="9">
-        <v>-245.55699999999999</v>
+        <v>-382.07799999999997</v>
       </c>
       <c r="J47" s="16">
         <f t="shared" si="0"/>
-        <v>2653.0115556435107</v>
-      </c>
-    </row>
-    <row r="48" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="49" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="50" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="51" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="52" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="53" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="54" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="55" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="56" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="57" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="58" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="59" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="60" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="61" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="62" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="63" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="64" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+        <v>2164.0650505114213</v>
+      </c>
+    </row>
+    <row r="48" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D48" s="46"/>
+      <c r="E48" s="9"/>
+      <c r="F48" s="9"/>
+      <c r="J48" s="47"/>
+    </row>
+    <row r="49" spans="4:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D49" s="46"/>
+      <c r="E49" s="9"/>
+      <c r="F49" s="9"/>
+      <c r="J49" s="47"/>
+    </row>
+    <row r="50" spans="4:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D50" s="46"/>
+      <c r="E50" s="9"/>
+      <c r="F50" s="9"/>
+      <c r="J50" s="47"/>
+    </row>
+    <row r="51" spans="4:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="52" spans="4:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="53" spans="4:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="54" spans="4:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="55" spans="4:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="56" spans="4:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="57" spans="4:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="58" spans="4:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="59" spans="4:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="60" spans="4:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="61" spans="4:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="62" spans="4:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="63" spans="4:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="64" spans="4:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="65" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="66" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="67" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -14213,7 +14202,7 @@
   </sheetPr>
   <dimension ref="A1:J1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+    <sheetView zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
       <selection activeCell="I15" sqref="I15"/>
     </sheetView>
   </sheetViews>
@@ -23923,8 +23912,8 @@
   </sheetPr>
   <dimension ref="A1:J1000"/>
   <sheetViews>
-    <sheetView topLeftCell="B3" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="G6" sqref="G6:I47"/>
+    <sheetView tabSelected="1" topLeftCell="B34" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="H48" sqref="H48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -24018,17 +24007,17 @@
         <v>20</v>
       </c>
       <c r="G6" s="9">
-        <v>54.887999999999998</v>
+        <v>171.34899999999999</v>
       </c>
       <c r="H6" s="9">
-        <v>87.793000000000006</v>
+        <v>218.98400000000001</v>
       </c>
       <c r="I6" s="9">
-        <v>28.045999999999999</v>
+        <v>90.122</v>
       </c>
       <c r="J6" s="16">
         <f t="shared" ref="J6:J47" si="0">SQRT(G6*G6+H6*H6+I6*I6)</f>
-        <v>107.27013335034128</v>
+        <v>292.29513670432493</v>
       </c>
     </row>
     <row r="7" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -24049,17 +24038,17 @@
         <v>20</v>
       </c>
       <c r="G7" s="9">
-        <v>-54.908999999999999</v>
+        <v>-171.249</v>
       </c>
       <c r="H7" s="9">
-        <v>263.48</v>
+        <v>328.22699999999998</v>
       </c>
       <c r="I7" s="9">
-        <v>84.171000000000006</v>
+        <v>135.244</v>
       </c>
       <c r="J7" s="16">
         <f t="shared" si="0"/>
-        <v>281.99550691810674</v>
+        <v>394.14479961810986</v>
       </c>
     </row>
     <row r="8" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -24080,17 +24069,17 @@
         <v>20</v>
       </c>
       <c r="G8" s="9">
-        <v>-9.1219999999999999</v>
+        <v>-23.201000000000001</v>
       </c>
       <c r="H8" s="9">
-        <v>60.814</v>
+        <v>72.501999999999995</v>
       </c>
       <c r="I8" s="9">
-        <v>0.45600000000000002</v>
+        <v>0.57999999999999996</v>
       </c>
       <c r="J8" s="16">
         <f t="shared" si="0"/>
-        <v>61.496027644068199</v>
+        <v>76.125966693369477</v>
       </c>
     </row>
     <row r="9" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -24111,17 +24100,17 @@
         <v>20</v>
       </c>
       <c r="G9" s="9">
-        <v>9.1129999999999995</v>
+        <v>23.109000000000002</v>
       </c>
       <c r="H9" s="9">
-        <v>20.25</v>
+        <v>48.143999999999998</v>
       </c>
       <c r="I9" s="9">
-        <v>0.152</v>
+        <v>0.38500000000000001</v>
       </c>
       <c r="J9" s="16">
         <f t="shared" si="0"/>
-        <v>22.206584001147046</v>
+        <v>53.404296100594756</v>
       </c>
     </row>
     <row r="10" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -24142,17 +24131,17 @@
         <v>35</v>
       </c>
       <c r="G10" s="9">
-        <v>54.887999999999998</v>
+        <v>171.34899999999999</v>
       </c>
       <c r="H10" s="9">
-        <v>87.793000000000006</v>
+        <v>218.98400000000001</v>
       </c>
       <c r="I10" s="9">
-        <v>28.045999999999999</v>
+        <v>90.122</v>
       </c>
       <c r="J10" s="16">
         <f t="shared" si="0"/>
-        <v>107.27013335034128</v>
+        <v>292.29513670432493</v>
       </c>
     </row>
     <row r="11" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -24173,17 +24162,17 @@
         <v>38</v>
       </c>
       <c r="G11" s="9">
-        <v>-54.908999999999999</v>
+        <v>-171.249</v>
       </c>
       <c r="H11" s="9">
-        <v>263.48</v>
+        <v>328.22699999999998</v>
       </c>
       <c r="I11" s="9">
-        <v>84.171000000000006</v>
+        <v>135.244</v>
       </c>
       <c r="J11" s="16">
         <f t="shared" si="0"/>
-        <v>281.99550691810674</v>
+        <v>394.14479961810986</v>
       </c>
     </row>
     <row r="12" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -24204,17 +24193,17 @@
         <v>40</v>
       </c>
       <c r="G12" s="9">
-        <v>-9.1219999999999999</v>
+        <v>-23.201000000000001</v>
       </c>
       <c r="H12" s="9">
-        <v>60.814</v>
+        <v>72.501999999999995</v>
       </c>
       <c r="I12" s="9">
-        <v>0.45600000000000002</v>
+        <v>0.57999999999999996</v>
       </c>
       <c r="J12" s="16">
         <f t="shared" si="0"/>
-        <v>61.496027644068199</v>
+        <v>76.125966693369477</v>
       </c>
     </row>
     <row r="13" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -24235,17 +24224,17 @@
         <v>42</v>
       </c>
       <c r="G13" s="9">
-        <v>9.1129999999999995</v>
+        <v>23.109000000000002</v>
       </c>
       <c r="H13" s="9">
-        <v>20.25</v>
+        <v>48.143999999999998</v>
       </c>
       <c r="I13" s="9">
-        <v>0.152</v>
+        <v>0.38500000000000001</v>
       </c>
       <c r="J13" s="16">
         <f t="shared" si="0"/>
-        <v>22.206584001147046</v>
+        <v>53.404296100594756</v>
       </c>
     </row>
     <row r="14" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -24266,17 +24255,17 @@
         <v>20</v>
       </c>
       <c r="G14" s="9">
-        <v>4.0000000000000001E-3</v>
+        <v>-8.9999999999999993E-3</v>
       </c>
       <c r="H14" s="9">
-        <v>2.7E-2</v>
+        <v>-2.9000000000000001E-2</v>
       </c>
       <c r="I14" s="9">
-        <v>2E-3</v>
+        <v>-2E-3</v>
       </c>
       <c r="J14" s="16">
         <f t="shared" si="0"/>
-        <v>2.7367864366808017E-2</v>
+        <v>3.043024810940588E-2</v>
       </c>
     </row>
     <row r="15" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -24297,17 +24286,17 @@
         <v>49</v>
       </c>
       <c r="G15" s="9">
-        <v>4.0000000000000001E-3</v>
+        <v>-8.9999999999999993E-3</v>
       </c>
       <c r="H15" s="9">
-        <v>2.7E-2</v>
+        <v>-2.9000000000000001E-2</v>
       </c>
       <c r="I15" s="9">
-        <v>2E-3</v>
+        <v>-2E-3</v>
       </c>
       <c r="J15" s="16">
         <f t="shared" si="0"/>
-        <v>2.7367864366808017E-2</v>
+        <v>3.043024810940588E-2</v>
       </c>
     </row>
     <row r="16" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -24328,17 +24317,17 @@
         <v>53</v>
       </c>
       <c r="G16" s="9">
-        <v>2.7E-2</v>
+        <v>0</v>
       </c>
       <c r="H16" s="9">
-        <v>-432.36399999999998</v>
+        <v>-667.82899999999995</v>
       </c>
       <c r="I16" s="9">
-        <v>148.16399999999999</v>
+        <v>209.73</v>
       </c>
       <c r="J16" s="16">
         <f t="shared" si="0"/>
-        <v>457.04616847863406</v>
+        <v>699.98731855727215</v>
       </c>
     </row>
     <row r="17" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -24359,17 +24348,17 @@
         <v>57</v>
       </c>
       <c r="G17" s="9">
-        <v>2.7E-2</v>
+        <v>0</v>
       </c>
       <c r="H17" s="9">
-        <v>-432.36399999999998</v>
+        <v>-667.82899999999995</v>
       </c>
       <c r="I17" s="9">
-        <v>148.16399999999999</v>
+        <v>209.73</v>
       </c>
       <c r="J17" s="16">
         <f t="shared" si="0"/>
-        <v>457.04616847863406</v>
+        <v>699.98731855727215</v>
       </c>
     </row>
     <row r="18" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -24393,14 +24382,14 @@
         <v>0</v>
       </c>
       <c r="H18" s="9">
-        <v>-313.17599999999999</v>
+        <v>-516.96900000000005</v>
       </c>
       <c r="I18" s="9">
-        <v>-83.688999999999993</v>
+        <v>-160.91</v>
       </c>
       <c r="J18" s="16">
         <f t="shared" si="0"/>
-        <v>324.16516730981442</v>
+        <v>541.43233654908352</v>
       </c>
     </row>
     <row r="19" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -24424,14 +24413,14 @@
         <v>0</v>
       </c>
       <c r="H19" s="9">
-        <v>-313.17599999999999</v>
+        <v>-516.96900000000005</v>
       </c>
       <c r="I19" s="9">
-        <v>-83.688999999999993</v>
+        <v>-160.91</v>
       </c>
       <c r="J19" s="16">
         <f t="shared" si="0"/>
-        <v>324.16516730981442</v>
+        <v>541.43233654908352</v>
       </c>
     </row>
     <row r="20" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -24452,17 +24441,17 @@
         <v>20</v>
       </c>
       <c r="G20" s="9">
-        <v>2.7E-2</v>
+        <v>0</v>
       </c>
       <c r="H20" s="9">
-        <v>-119.188</v>
+        <v>-150.86000000000001</v>
       </c>
       <c r="I20" s="9">
-        <v>231.85300000000001</v>
+        <v>370.64100000000002</v>
       </c>
       <c r="J20" s="16">
         <f t="shared" si="0"/>
-        <v>260.69444505397502</v>
+        <v>400.16682831164309</v>
       </c>
     </row>
     <row r="21" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -24489,11 +24478,11 @@
         <v>0</v>
       </c>
       <c r="I21" s="9">
-        <v>260.99099999999999</v>
+        <v>436.05900000000003</v>
       </c>
       <c r="J21" s="16">
         <f t="shared" si="0"/>
-        <v>260.99099999999999</v>
+        <v>436.05900000000003</v>
       </c>
     </row>
     <row r="22" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -24520,11 +24509,11 @@
         <v>0</v>
       </c>
       <c r="I22" s="9">
-        <v>1.4999999999999999E-2</v>
+        <v>2.5000000000000001E-2</v>
       </c>
       <c r="J22" s="16">
         <f t="shared" si="0"/>
-        <v>1.4999999999999999E-2</v>
+        <v>2.5000000000000001E-2</v>
       </c>
     </row>
     <row r="23" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -24551,11 +24540,11 @@
         <v>0</v>
       </c>
       <c r="I23" s="9">
-        <v>212.49100000000001</v>
+        <v>355.02600000000001</v>
       </c>
       <c r="J23" s="16">
         <f t="shared" si="0"/>
-        <v>212.49100000000001</v>
+        <v>355.02600000000001</v>
       </c>
     </row>
     <row r="24" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -24582,11 +24571,11 @@
         <v>0</v>
       </c>
       <c r="I24" s="9">
-        <v>48.485999999999997</v>
+        <v>81.007999999999996</v>
       </c>
       <c r="J24" s="16">
         <f t="shared" si="0"/>
-        <v>48.485999999999997</v>
+        <v>81.007999999999996</v>
       </c>
     </row>
     <row r="25" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -24640,17 +24629,17 @@
         <v>20</v>
       </c>
       <c r="G26" s="9">
-        <v>-1006.436</v>
+        <v>-1043.3219999999999</v>
       </c>
       <c r="H26" s="9">
-        <v>-2585.2159999999999</v>
+        <v>-2471.3780000000002</v>
       </c>
       <c r="I26" s="9">
-        <v>139.02099999999999</v>
+        <v>136.928</v>
       </c>
       <c r="J26" s="16">
         <f t="shared" si="0"/>
-        <v>2777.6936525097581</v>
+        <v>2686.0713489689733</v>
       </c>
     </row>
     <row r="27" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -24671,17 +24660,17 @@
         <v>20</v>
       </c>
       <c r="G27" s="9">
-        <v>-180.15299999999999</v>
+        <v>-111.401</v>
       </c>
       <c r="H27" s="9">
-        <v>462.46</v>
+        <v>254.80500000000001</v>
       </c>
       <c r="I27" s="9">
-        <v>-24.869</v>
+        <v>-14.611000000000001</v>
       </c>
       <c r="J27" s="16">
         <f t="shared" si="0"/>
-        <v>496.9334182463482</v>
+        <v>278.47666355908535</v>
       </c>
     </row>
     <row r="28" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -24702,17 +24691,17 @@
         <v>20</v>
       </c>
       <c r="G28" s="9">
-        <v>1635.364</v>
+        <v>1627.2059999999999</v>
       </c>
       <c r="H28" s="9">
-        <v>-4239.6819999999998</v>
+        <v>-4218.5320000000002</v>
       </c>
       <c r="I28" s="9">
-        <v>468.57499999999999</v>
+        <v>466.238</v>
       </c>
       <c r="J28" s="16">
         <f t="shared" si="0"/>
-        <v>4568.2470822236619</v>
+        <v>4545.4581148773113</v>
       </c>
     </row>
     <row r="29" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -24733,17 +24722,17 @@
         <v>20</v>
       </c>
       <c r="G29" s="9">
-        <v>1879.5350000000001</v>
+        <v>1766.76</v>
       </c>
       <c r="H29" s="9">
-        <v>5078.3490000000002</v>
+        <v>4773.6409999999996</v>
       </c>
       <c r="I29" s="9">
-        <v>-561.26599999999996</v>
+        <v>-527.58900000000006</v>
       </c>
       <c r="J29" s="16">
         <f t="shared" si="0"/>
-        <v>5444.015053688041</v>
+        <v>5117.3664562352769</v>
       </c>
     </row>
     <row r="30" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -24764,17 +24753,17 @@
         <v>99</v>
       </c>
       <c r="G30" s="9">
-        <v>1879.5350000000001</v>
+        <v>1766.76</v>
       </c>
       <c r="H30" s="9">
-        <v>5078.3490000000002</v>
+        <v>4773.6409999999996</v>
       </c>
       <c r="I30" s="9">
-        <v>-561.26599999999996</v>
+        <v>-527.58900000000006</v>
       </c>
       <c r="J30" s="16">
         <f t="shared" si="0"/>
-        <v>5444.015053688041</v>
+        <v>5117.3664562352769</v>
       </c>
     </row>
     <row r="31" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -24795,17 +24784,17 @@
         <v>101</v>
       </c>
       <c r="G31" s="9">
-        <v>1635.364</v>
+        <v>1627.2059999999999</v>
       </c>
       <c r="H31" s="9">
-        <v>-4239.6819999999998</v>
+        <v>-4218.5320000000002</v>
       </c>
       <c r="I31" s="9">
-        <v>468.57499999999999</v>
+        <v>466.238</v>
       </c>
       <c r="J31" s="16">
         <f t="shared" si="0"/>
-        <v>4568.2470822236619</v>
+        <v>4545.4581148773113</v>
       </c>
     </row>
     <row r="32" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -24826,17 +24815,17 @@
         <v>103</v>
       </c>
       <c r="G32" s="9">
-        <v>-180.15299999999999</v>
+        <v>-111.401</v>
       </c>
       <c r="H32" s="9">
-        <v>462.46</v>
+        <v>254.80500000000001</v>
       </c>
       <c r="I32" s="9">
-        <v>-24.869</v>
+        <v>-14.611000000000001</v>
       </c>
       <c r="J32" s="16">
         <f t="shared" si="0"/>
-        <v>496.9334182463482</v>
+        <v>278.47666355908535</v>
       </c>
     </row>
     <row r="33" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -24857,17 +24846,17 @@
         <v>105</v>
       </c>
       <c r="G33" s="9">
-        <v>-1006.436</v>
+        <v>-1043.3219999999999</v>
       </c>
       <c r="H33" s="9">
-        <v>-2585.2159999999999</v>
+        <v>-2471.3780000000002</v>
       </c>
       <c r="I33" s="9">
-        <v>139.02099999999999</v>
+        <v>136.928</v>
       </c>
       <c r="J33" s="16">
         <f t="shared" si="0"/>
-        <v>2777.6936525097581</v>
+        <v>2686.0713489689733</v>
       </c>
     </row>
     <row r="34" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -24891,14 +24880,14 @@
         <v>0</v>
       </c>
       <c r="H34" s="9">
-        <v>1895.4960000000001</v>
+        <v>1687.787</v>
       </c>
       <c r="I34" s="9">
-        <v>1356.751</v>
+        <v>1620.356</v>
       </c>
       <c r="J34" s="16">
         <f t="shared" si="0"/>
-        <v>2331.0251740418848</v>
+        <v>2339.6962461193548</v>
       </c>
     </row>
     <row r="35" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -24922,14 +24911,14 @@
         <v>0</v>
       </c>
       <c r="H35" s="9">
-        <v>1895.4960000000001</v>
+        <v>1687.787</v>
       </c>
       <c r="I35" s="9">
-        <v>1356.751</v>
+        <v>1620.356</v>
       </c>
       <c r="J35" s="16">
         <f t="shared" si="0"/>
-        <v>2331.0251740418848</v>
+        <v>2339.6962461193548</v>
       </c>
     </row>
     <row r="36" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -24953,14 +24942,14 @@
         <v>0</v>
       </c>
       <c r="H36" s="9">
-        <v>-158.00200000000001</v>
+        <v>-247.084</v>
       </c>
       <c r="I36" s="9">
-        <v>1547.6379999999999</v>
+        <v>1967.42</v>
       </c>
       <c r="J36" s="16">
         <f t="shared" si="0"/>
-        <v>1555.6824904356286</v>
+        <v>1982.8746706375571</v>
       </c>
     </row>
     <row r="37" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -24984,14 +24973,14 @@
         <v>0</v>
       </c>
       <c r="H37" s="9">
-        <v>-158.00200000000001</v>
+        <v>-247.084</v>
       </c>
       <c r="I37" s="9">
-        <v>1547.6379999999999</v>
+        <v>1967.42</v>
       </c>
       <c r="J37" s="16">
         <f t="shared" si="0"/>
-        <v>1555.6824904356286</v>
+        <v>1982.8746706375571</v>
       </c>
     </row>
     <row r="38" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -25012,17 +25001,17 @@
         <v>119</v>
       </c>
       <c r="G38" s="9">
-        <v>6.2990000000000004</v>
+        <v>0.27100000000000002</v>
       </c>
       <c r="H38" s="9">
-        <v>-611.40800000000002</v>
+        <v>-26.323</v>
       </c>
       <c r="I38" s="9">
-        <v>60.793999999999997</v>
+        <v>2.617</v>
       </c>
       <c r="J38" s="16">
         <f t="shared" si="0"/>
-        <v>614.45531188280893</v>
+        <v>26.454157688348349</v>
       </c>
     </row>
     <row r="39" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -25043,17 +25032,17 @@
         <v>20</v>
       </c>
       <c r="G39" s="9">
-        <v>6.2990000000000004</v>
+        <v>0.27100000000000002</v>
       </c>
       <c r="H39" s="9">
-        <v>-611.40800000000002</v>
+        <v>-26.323</v>
       </c>
       <c r="I39" s="9">
-        <v>60.793999999999997</v>
+        <v>2.617</v>
       </c>
       <c r="J39" s="16">
         <f t="shared" si="0"/>
-        <v>614.45531188280893</v>
+        <v>26.454157688348349</v>
       </c>
     </row>
     <row r="40" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -25080,11 +25069,11 @@
         <v>0</v>
       </c>
       <c r="I40" s="9">
-        <v>260.995</v>
+        <v>436.06400000000002</v>
       </c>
       <c r="J40" s="16">
         <f t="shared" si="0"/>
-        <v>260.995</v>
+        <v>436.06400000000002</v>
       </c>
     </row>
     <row r="41" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -25111,11 +25100,11 @@
         <v>0</v>
       </c>
       <c r="I41" s="9">
-        <v>1439.0070000000001</v>
+        <v>1683.9380000000001</v>
       </c>
       <c r="J41" s="16">
         <f t="shared" si="0"/>
-        <v>1439.0070000000001</v>
+        <v>1683.9380000000001</v>
       </c>
     </row>
     <row r="42" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -25142,11 +25131,11 @@
         <v>0</v>
       </c>
       <c r="I42" s="9">
-        <v>1439.0070000000001</v>
+        <v>1683.9380000000001</v>
       </c>
       <c r="J42" s="16">
         <f t="shared" si="0"/>
-        <v>1439.0070000000001</v>
+        <v>1683.9380000000001</v>
       </c>
     </row>
     <row r="43" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -25167,17 +25156,17 @@
         <v>126</v>
       </c>
       <c r="G43" s="9">
-        <v>408.048</v>
+        <v>391.43</v>
       </c>
       <c r="H43" s="9">
-        <v>76.503</v>
+        <v>70.941000000000003</v>
       </c>
       <c r="I43" s="9">
-        <v>-1637.8979999999999</v>
+        <v>-1518.817</v>
       </c>
       <c r="J43" s="16">
         <f t="shared" si="0"/>
-        <v>1689.6939775346896</v>
+        <v>1570.0494100091246</v>
       </c>
     </row>
     <row r="44" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -25198,17 +25187,17 @@
         <v>126</v>
       </c>
       <c r="G44" s="9">
-        <v>1926.5530000000001</v>
+        <v>1848.078</v>
       </c>
       <c r="H44" s="9">
-        <v>118.389</v>
+        <v>101.872</v>
       </c>
       <c r="I44" s="9">
-        <v>-2533.6350000000002</v>
+        <v>-2180.009</v>
       </c>
       <c r="J44" s="16">
         <f t="shared" si="0"/>
-        <v>3185.1104738069921</v>
+        <v>2859.7568845181581</v>
       </c>
     </row>
     <row r="45" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -25229,17 +25218,17 @@
         <v>126</v>
       </c>
       <c r="G45" s="9">
-        <v>7.0000000000000001E-3</v>
+        <v>6.0000000000000001E-3</v>
       </c>
       <c r="H45" s="9">
-        <v>-194.892</v>
+        <v>-172.81399999999999</v>
       </c>
       <c r="I45" s="9">
-        <v>-9.1010000000000009</v>
+        <v>-8.07</v>
       </c>
       <c r="J45" s="16">
         <f t="shared" si="0"/>
-        <v>195.1043820984039</v>
+        <v>173.00232233123344</v>
       </c>
     </row>
     <row r="46" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -25266,11 +25255,11 @@
         <v>0</v>
       </c>
       <c r="I46" s="9">
-        <v>5619.6419999999998</v>
+        <v>5390.8339999999998</v>
       </c>
       <c r="J46" s="16">
         <f t="shared" si="0"/>
-        <v>5619.6419999999998</v>
+        <v>5390.8339999999998</v>
       </c>
     </row>
     <row r="47" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -25294,14 +25283,14 @@
         <v>0</v>
       </c>
       <c r="H47" s="9">
-        <v>2053.498</v>
+        <v>1934.8710000000001</v>
       </c>
       <c r="I47" s="9">
-        <v>-190.887</v>
+        <v>-347.065</v>
       </c>
       <c r="J47" s="16">
         <f t="shared" si="0"/>
-        <v>2062.3510571124889</v>
+        <v>1965.751739377585</v>
       </c>
     </row>
     <row r="48" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
màj cas de charge
Bump 3g et Right turn 2.2g
</commit_message>
<xml_diff>
--- a/SU_Suspension/13_Cas_de_charges/Cas de charges Invictus.xlsx
+++ b/SU_Suspension/13_Cas_de_charges/Cas de charges Invictus.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Martin Kawczynski\Documents\EPSA\GIT\STUF-2020\SU_Suspension\13_Cas_de_charges\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0C8E69EB-B7CD-49F9-81AC-8D2A4BFAE9E0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B6EE3800-C64C-4AD0-B28C-459350DA2307}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="857" firstSheet="3" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="857" firstSheet="3" activeTab="10" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Presentation" sheetId="1" r:id="rId1"/>
@@ -1143,72 +1143,6 @@
         <left style="thin">
           <color indexed="64"/>
         </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
         <right/>
         <top style="thin">
           <color indexed="64"/>
@@ -2864,6 +2798,72 @@
           <color indexed="64"/>
         </left>
         <right/>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
         <top style="thin">
           <color indexed="64"/>
         </top>
@@ -3847,15 +3847,15 @@
 </file>
 
 <file path=xl/tables/table10.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{00000000-000C-0000-FFFF-FFFF04000000}" name="Table_226" displayName="Table_226" ref="D5:J50" headerRowDxfId="37" totalsRowDxfId="36">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{00000000-000C-0000-FFFF-FFFF04000000}" name="Table_226" displayName="Table_226" ref="D5:J50" headerRowDxfId="34" totalsRowDxfId="33">
   <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0400-000001000000}" name="Type" dataDxfId="35"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0400-000002000000}" name="Part 1" dataDxfId="34"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0400-000003000000}" name="Part 2" dataDxfId="33"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0400-000004000000}" name="Rx" dataDxfId="32"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0400-000005000000}" name="Ry" dataDxfId="31"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0400-000006000000}" name="Rz" dataDxfId="30"/>
-    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0400-00000A000000}" name="F" dataDxfId="29">
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0400-000001000000}" name="Type" dataDxfId="32"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0400-000002000000}" name="Part 1" dataDxfId="31"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0400-000003000000}" name="Part 2" dataDxfId="30"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0400-000004000000}" name="Rx" dataDxfId="29"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0400-000005000000}" name="Ry" dataDxfId="28"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0400-000006000000}" name="Rz" dataDxfId="27"/>
+    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0400-00000A000000}" name="F" dataDxfId="26">
       <calculatedColumnFormula>SQRT(G6*G6+H6*H6+I6*I6)</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -3864,15 +3864,15 @@
 </file>
 
 <file path=xl/tables/table11.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="9" xr:uid="{00000000-000C-0000-FFFF-FFFF05000000}" name="Table_22910" displayName="Table_22910" ref="D5:J48" headerRowDxfId="28" totalsRowDxfId="27">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="9" xr:uid="{00000000-000C-0000-FFFF-FFFF05000000}" name="Table_22910" displayName="Table_22910" ref="D5:J48" headerRowDxfId="25" totalsRowDxfId="24">
   <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0500-000001000000}" name="Type" dataDxfId="26"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0500-000002000000}" name="Part 1" dataDxfId="25"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0500-000003000000}" name="Part 2" dataDxfId="24"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0500-000004000000}" name="Rx" dataDxfId="23"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0500-000005000000}" name="Ry" dataDxfId="22"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0500-000006000000}" name="Rz" dataDxfId="21"/>
-    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0500-00000A000000}" name="F" dataDxfId="20">
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0500-000001000000}" name="Type" dataDxfId="23"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0500-000002000000}" name="Part 1" dataDxfId="22"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0500-000003000000}" name="Part 2" dataDxfId="21"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0500-000004000000}" name="Rx" dataDxfId="20"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0500-000005000000}" name="Ry" dataDxfId="19"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0500-000006000000}" name="Rz" dataDxfId="18"/>
+    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0500-00000A000000}" name="F" dataDxfId="17">
       <calculatedColumnFormula>SQRT(G6*G6+H6*H6+I6*I6)</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -3881,29 +3881,29 @@
 </file>
 
 <file path=xl/tables/table12.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="11" xr:uid="{00000000-000C-0000-FFFF-FFFF06000000}" name="Table_229101112" displayName="Table_229101112" ref="D5:I50" headerRowDxfId="19" totalsRowDxfId="18">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="11" xr:uid="{00000000-000C-0000-FFFF-FFFF06000000}" name="Table_229101112" displayName="Table_229101112" ref="D5:I50" headerRowDxfId="16" totalsRowDxfId="15">
   <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0600-000001000000}" name="Type" dataDxfId="17"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0600-000002000000}" name="Part 1" dataDxfId="16"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0600-000003000000}" name="Part 2" dataDxfId="15"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0600-000004000000}" name="Rx" dataDxfId="14"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0600-000005000000}" name="Ry" dataDxfId="13"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0600-000006000000}" name="Rz" dataDxfId="12"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0600-000001000000}" name="Type" dataDxfId="14"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0600-000002000000}" name="Part 1" dataDxfId="13"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0600-000003000000}" name="Part 2" dataDxfId="12"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0600-000004000000}" name="Rx" dataDxfId="11"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0600-000005000000}" name="Ry" dataDxfId="10"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0600-000006000000}" name="Rz" dataDxfId="9"/>
   </tableColumns>
   <tableStyleInfo name="BRAKING 2G-style" showFirstColumn="1" showLastColumn="1" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table13.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="12" xr:uid="{00000000-000C-0000-FFFF-FFFF07000000}" name="Table_22910111213" displayName="Table_22910111213" ref="D5:J47" headerRowDxfId="11" totalsRowDxfId="10">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="12" xr:uid="{00000000-000C-0000-FFFF-FFFF07000000}" name="Table_22910111213" displayName="Table_22910111213" ref="D5:J47" headerRowDxfId="8" totalsRowDxfId="7">
   <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0700-000001000000}" name="Type" dataDxfId="9"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0700-000002000000}" name="Part 1" dataDxfId="8"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0700-000003000000}" name="Part 2" dataDxfId="7"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0700-000004000000}" name="Rx" dataDxfId="6"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0700-000005000000}" name="Ry" dataDxfId="5"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0700-000006000000}" name="Rz" dataDxfId="4"/>
-    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0700-00000A000000}" name="F" dataDxfId="3">
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0700-000001000000}" name="Type" dataDxfId="6"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0700-000002000000}" name="Part 1" dataDxfId="5"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0700-000003000000}" name="Part 2" dataDxfId="4"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0700-000004000000}" name="Rx" dataDxfId="3"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0700-000005000000}" name="Ry" dataDxfId="2"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0700-000006000000}" name="Rz" dataDxfId="1"/>
+    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0700-00000A000000}" name="F" dataDxfId="0">
       <calculatedColumnFormula>SQRT(G6*G6+H6*H6+I6*I6)</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -3951,10 +3951,10 @@
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0200-000001000000}" name="Type" dataDxfId="86"/>
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0200-000002000000}" name="Part 1" dataDxfId="85"/>
     <tableColumn id="3" xr3:uid="{00000000-0010-0000-0200-000003000000}" name="Part 2" dataDxfId="84"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0200-000004000000}" name="Rx" dataDxfId="2"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0200-000005000000}" name="Ry" dataDxfId="1"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0200-000006000000}" name="Rz" dataDxfId="0"/>
-    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0200-00000A000000}" name="F" dataDxfId="83">
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0200-000004000000}" name="Rx" dataDxfId="83"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0200-000005000000}" name="Ry" dataDxfId="82"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0200-000006000000}" name="Rz" dataDxfId="81"/>
+    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0200-00000A000000}" name="F" dataDxfId="80">
       <calculatedColumnFormula>SQRT(G6*G6+H6*H6+I6*I6)</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -3963,15 +3963,15 @@
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="13" xr:uid="{B0AFE184-AE6C-4FF3-8D63-F0BC8E23A6CF}" name="Table_2295814" displayName="Table_2295814" ref="D5:J50" headerRowDxfId="82" totalsRowDxfId="81">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="13" xr:uid="{B0AFE184-AE6C-4FF3-8D63-F0BC8E23A6CF}" name="Table_2295814" displayName="Table_2295814" ref="D5:J50" headerRowDxfId="79" totalsRowDxfId="78">
   <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{5CF42B42-17BB-4840-A98E-B5C21DA88B45}" name="Type" dataDxfId="80"/>
-    <tableColumn id="2" xr3:uid="{CA484149-8619-432A-AAEE-273B43A77EEB}" name="Part 1" dataDxfId="79"/>
-    <tableColumn id="3" xr3:uid="{153A0EC0-A7FA-4356-B034-40ABDE58108F}" name="Part 2" dataDxfId="78"/>
-    <tableColumn id="4" xr3:uid="{6438DE58-B6AF-4E59-A3B4-304BF0284DF3}" name="Rx" dataDxfId="77"/>
-    <tableColumn id="5" xr3:uid="{11464FEA-AD23-45DD-8207-9270CBF74988}" name="Ry" dataDxfId="76"/>
-    <tableColumn id="6" xr3:uid="{832F0331-1E22-477B-8D82-FCD2E083B4C0}" name="Rz" dataDxfId="75"/>
-    <tableColumn id="10" xr3:uid="{E2A35E5D-E1C6-41C4-A510-2FF34E76A089}" name="F" dataDxfId="74">
+    <tableColumn id="1" xr3:uid="{5CF42B42-17BB-4840-A98E-B5C21DA88B45}" name="Type" dataDxfId="77"/>
+    <tableColumn id="2" xr3:uid="{CA484149-8619-432A-AAEE-273B43A77EEB}" name="Part 1" dataDxfId="76"/>
+    <tableColumn id="3" xr3:uid="{153A0EC0-A7FA-4356-B034-40ABDE58108F}" name="Part 2" dataDxfId="75"/>
+    <tableColumn id="4" xr3:uid="{6438DE58-B6AF-4E59-A3B4-304BF0284DF3}" name="Rx" dataDxfId="74"/>
+    <tableColumn id="5" xr3:uid="{11464FEA-AD23-45DD-8207-9270CBF74988}" name="Ry" dataDxfId="73"/>
+    <tableColumn id="6" xr3:uid="{832F0331-1E22-477B-8D82-FCD2E083B4C0}" name="Rz" dataDxfId="72"/>
+    <tableColumn id="10" xr3:uid="{E2A35E5D-E1C6-41C4-A510-2FF34E76A089}" name="F" dataDxfId="71">
       <calculatedColumnFormula>SQRT(G6*G6+H6*H6+I6*I6)</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -3980,15 +3980,15 @@
 </file>
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{63497B11-6CFB-431E-8043-C5EA4856B019}" name="Table_22958" displayName="Table_22958" ref="D5:J50" headerRowDxfId="73" totalsRowDxfId="72">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{63497B11-6CFB-431E-8043-C5EA4856B019}" name="Table_22958" displayName="Table_22958" ref="D5:J50" headerRowDxfId="70" totalsRowDxfId="69">
   <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{C7C2A27F-B68F-4595-B3A6-80824AAEBE7E}" name="Type" dataDxfId="71"/>
-    <tableColumn id="2" xr3:uid="{F9164B72-0BB0-4A2B-AB4C-E9D021461BC3}" name="Part 1" dataDxfId="70"/>
-    <tableColumn id="3" xr3:uid="{E1FE5AA7-DF77-4186-B6D1-FCD4A338577B}" name="Part 2" dataDxfId="69"/>
-    <tableColumn id="4" xr3:uid="{E98E1800-10A5-4E7A-902F-83A63939A99C}" name="Rx" dataDxfId="68"/>
-    <tableColumn id="5" xr3:uid="{DF57FFDE-C9BB-4026-9267-B35746E5617B}" name="Ry" dataDxfId="67"/>
-    <tableColumn id="6" xr3:uid="{B76AC1C2-BF2D-435A-BC8A-DF791C33A631}" name="Rz" dataDxfId="66"/>
-    <tableColumn id="10" xr3:uid="{B94DD169-5874-4A11-82AB-41D75CE9E1C4}" name="F" dataDxfId="65">
+    <tableColumn id="1" xr3:uid="{C7C2A27F-B68F-4595-B3A6-80824AAEBE7E}" name="Type" dataDxfId="68"/>
+    <tableColumn id="2" xr3:uid="{F9164B72-0BB0-4A2B-AB4C-E9D021461BC3}" name="Part 1" dataDxfId="67"/>
+    <tableColumn id="3" xr3:uid="{E1FE5AA7-DF77-4186-B6D1-FCD4A338577B}" name="Part 2" dataDxfId="66"/>
+    <tableColumn id="4" xr3:uid="{E98E1800-10A5-4E7A-902F-83A63939A99C}" name="Rx" dataDxfId="65"/>
+    <tableColumn id="5" xr3:uid="{DF57FFDE-C9BB-4026-9267-B35746E5617B}" name="Ry" dataDxfId="64"/>
+    <tableColumn id="6" xr3:uid="{B76AC1C2-BF2D-435A-BC8A-DF791C33A631}" name="Rz" dataDxfId="63"/>
+    <tableColumn id="10" xr3:uid="{B94DD169-5874-4A11-82AB-41D75CE9E1C4}" name="F" dataDxfId="62">
       <calculatedColumnFormula>SQRT(G6*G6+H6*H6+I6*I6)</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -3997,15 +3997,15 @@
 </file>
 
 <file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{EEA5A4BA-6E68-456A-BA37-768ED05DFF03}" name="Table_2295" displayName="Table_2295" ref="D5:J50" headerRowDxfId="64" totalsRowDxfId="63">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{EEA5A4BA-6E68-456A-BA37-768ED05DFF03}" name="Table_2295" displayName="Table_2295" ref="D5:J50" headerRowDxfId="61" totalsRowDxfId="60">
   <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{0C6F79C5-B10E-4271-A5D4-4408A2063025}" name="Type" dataDxfId="62"/>
-    <tableColumn id="2" xr3:uid="{E86F6686-943D-4BC7-9D6F-FA4449FBAA83}" name="Part 1" dataDxfId="61"/>
-    <tableColumn id="3" xr3:uid="{2D13C6D0-4244-4392-980F-76660A4A5060}" name="Part 2" dataDxfId="60"/>
-    <tableColumn id="4" xr3:uid="{064AD1C3-3244-488D-BBFE-2B8CCB4B6B60}" name="Rx" dataDxfId="59"/>
-    <tableColumn id="5" xr3:uid="{7E162B99-B799-4078-9949-6F27B23EC330}" name="Ry" dataDxfId="58"/>
-    <tableColumn id="6" xr3:uid="{673CB13C-8584-493A-B7B1-E54129F7F8A7}" name="Rz" dataDxfId="57"/>
-    <tableColumn id="10" xr3:uid="{54734AB4-F9C8-4F27-8D94-075B17BBB2D5}" name="F" dataDxfId="56">
+    <tableColumn id="1" xr3:uid="{0C6F79C5-B10E-4271-A5D4-4408A2063025}" name="Type" dataDxfId="59"/>
+    <tableColumn id="2" xr3:uid="{E86F6686-943D-4BC7-9D6F-FA4449FBAA83}" name="Part 1" dataDxfId="58"/>
+    <tableColumn id="3" xr3:uid="{2D13C6D0-4244-4392-980F-76660A4A5060}" name="Part 2" dataDxfId="57"/>
+    <tableColumn id="4" xr3:uid="{064AD1C3-3244-488D-BBFE-2B8CCB4B6B60}" name="Rx" dataDxfId="56"/>
+    <tableColumn id="5" xr3:uid="{7E162B99-B799-4078-9949-6F27B23EC330}" name="Ry" dataDxfId="55"/>
+    <tableColumn id="6" xr3:uid="{673CB13C-8584-493A-B7B1-E54129F7F8A7}" name="Rz" dataDxfId="54"/>
+    <tableColumn id="10" xr3:uid="{54734AB4-F9C8-4F27-8D94-075B17BBB2D5}" name="F" dataDxfId="53">
       <calculatedColumnFormula>SQRT(G6*G6+H6*H6+I6*I6)</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -4014,15 +4014,15 @@
 </file>
 
 <file path=xl/tables/table8.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{D0C05053-3AE3-4D2D-9A69-48FE95801512}" name="Table_2297" displayName="Table_2297" ref="D2:J47" headerRowDxfId="55" totalsRowDxfId="54">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{D0C05053-3AE3-4D2D-9A69-48FE95801512}" name="Table_2297" displayName="Table_2297" ref="D2:J47" headerRowDxfId="52" totalsRowDxfId="51">
   <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{817511AE-EF59-4237-8AC4-BD3087668C1E}" name="Type" dataDxfId="53"/>
-    <tableColumn id="2" xr3:uid="{C5BA019C-B66B-499C-AB50-D0EE858D989B}" name="Part 1" dataDxfId="52"/>
-    <tableColumn id="3" xr3:uid="{734CB3FF-2256-439B-B403-9C5DE48737CB}" name="Part 2" dataDxfId="51"/>
-    <tableColumn id="4" xr3:uid="{E2A78AA9-3F71-4A43-8FD5-ABAEC128EA00}" name="Rx" dataDxfId="50"/>
-    <tableColumn id="5" xr3:uid="{2E02113B-8D48-42B2-ABCD-F2B6F3E2A60B}" name="Ry" dataDxfId="49"/>
-    <tableColumn id="6" xr3:uid="{055EC799-14EC-445A-A1B5-BEFABF90C4C5}" name="Rz" dataDxfId="48"/>
-    <tableColumn id="10" xr3:uid="{23D90AD4-2234-478E-9B30-A06F6533CDD2}" name="F" dataDxfId="47">
+    <tableColumn id="1" xr3:uid="{817511AE-EF59-4237-8AC4-BD3087668C1E}" name="Type" dataDxfId="50"/>
+    <tableColumn id="2" xr3:uid="{C5BA019C-B66B-499C-AB50-D0EE858D989B}" name="Part 1" dataDxfId="49"/>
+    <tableColumn id="3" xr3:uid="{734CB3FF-2256-439B-B403-9C5DE48737CB}" name="Part 2" dataDxfId="48"/>
+    <tableColumn id="4" xr3:uid="{E2A78AA9-3F71-4A43-8FD5-ABAEC128EA00}" name="Rx" dataDxfId="47"/>
+    <tableColumn id="5" xr3:uid="{2E02113B-8D48-42B2-ABCD-F2B6F3E2A60B}" name="Ry" dataDxfId="46"/>
+    <tableColumn id="6" xr3:uid="{055EC799-14EC-445A-A1B5-BEFABF90C4C5}" name="Rz" dataDxfId="45"/>
+    <tableColumn id="10" xr3:uid="{23D90AD4-2234-478E-9B30-A06F6533CDD2}" name="F" dataDxfId="44">
       <calculatedColumnFormula>SQRT(G3*G3+H3*H3+I3*I3)</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -4031,15 +4031,15 @@
 </file>
 
 <file path=xl/tables/table9.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{00000000-000C-0000-FFFF-FFFF03000000}" name="Table_229" displayName="Table_229" ref="D5:J50" headerRowDxfId="46" totalsRowDxfId="45">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{00000000-000C-0000-FFFF-FFFF03000000}" name="Table_229" displayName="Table_229" ref="D5:J50" headerRowDxfId="43" totalsRowDxfId="42">
   <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0300-000001000000}" name="Type" dataDxfId="44"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0300-000002000000}" name="Part 1" dataDxfId="43"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0300-000003000000}" name="Part 2" dataDxfId="42"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0300-000004000000}" name="Rx" dataDxfId="41"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0300-000005000000}" name="Ry" dataDxfId="40"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0300-000006000000}" name="Rz" dataDxfId="39"/>
-    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0300-00000A000000}" name="F" dataDxfId="38">
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0300-000001000000}" name="Type" dataDxfId="41"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0300-000002000000}" name="Part 1" dataDxfId="40"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0300-000003000000}" name="Part 2" dataDxfId="39"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0300-000004000000}" name="Rx" dataDxfId="38"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0300-000005000000}" name="Ry" dataDxfId="37"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0300-000006000000}" name="Rz" dataDxfId="36"/>
+    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0300-00000A000000}" name="F" dataDxfId="35">
       <calculatedColumnFormula>SQRT(G6*G6+H6*H6+I6*I6)</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -7968,8 +7968,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:J50"/>
   <sheetViews>
-    <sheetView zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="O27" sqref="O27"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="N36" sqref="N36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8062,17 +8062,17 @@
         <v>20</v>
       </c>
       <c r="G6" s="9">
-        <v>591.23699999999997</v>
+        <v>1104.7070000000001</v>
       </c>
       <c r="H6" s="9">
-        <v>945.678</v>
+        <v>1411.818</v>
       </c>
       <c r="I6" s="9">
-        <v>302.10399999999998</v>
+        <v>581.02800000000002</v>
       </c>
       <c r="J6" s="16">
         <f t="shared" ref="J6:J47" si="0">SQRT(G6*G6+H6*H6+I6*I6)</f>
-        <v>1155.4803748523814</v>
+        <v>1884.4630953555445</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
@@ -8093,17 +8093,17 @@
         <v>20</v>
       </c>
       <c r="G7" s="9">
-        <v>-591.46600000000001</v>
+        <v>-1104.06</v>
       </c>
       <c r="H7" s="9">
-        <v>2838.1260000000002</v>
+        <v>2116.1149999999998</v>
       </c>
       <c r="I7" s="9">
-        <v>906.66</v>
+        <v>871.93100000000004</v>
       </c>
       <c r="J7" s="16">
         <f t="shared" si="0"/>
-        <v>3037.5686949651031</v>
+        <v>2541.0932382708825</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
@@ -8124,17 +8124,17 @@
         <v>20</v>
       </c>
       <c r="G8" s="9">
-        <v>-98.260999999999996</v>
+        <v>-149.577</v>
       </c>
       <c r="H8" s="9">
-        <v>655.07299999999998</v>
+        <v>467.428</v>
       </c>
       <c r="I8" s="9">
-        <v>4.9130000000000003</v>
+        <v>3.7389999999999999</v>
       </c>
       <c r="J8" s="16">
         <f t="shared" si="0"/>
-        <v>662.41980421708399</v>
+        <v>490.79139584348866</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
@@ -8155,17 +8155,17 @@
         <v>20</v>
       </c>
       <c r="G9" s="9">
-        <v>98.156999999999996</v>
+        <v>148.98599999999999</v>
       </c>
       <c r="H9" s="9">
-        <v>218.12700000000001</v>
+        <v>310.38799999999998</v>
       </c>
       <c r="I9" s="9">
-        <v>1.6359999999999999</v>
+        <v>2.4830000000000001</v>
       </c>
       <c r="J9" s="16">
         <f t="shared" si="0"/>
-        <v>239.20046252881704</v>
+        <v>344.30176303498649</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
@@ -8186,17 +8186,17 @@
         <v>35</v>
       </c>
       <c r="G10" s="9">
-        <v>591.23699999999997</v>
+        <v>1104.7070000000001</v>
       </c>
       <c r="H10" s="9">
-        <v>945.678</v>
+        <v>1411.818</v>
       </c>
       <c r="I10" s="9">
-        <v>302.10399999999998</v>
+        <v>581.02800000000002</v>
       </c>
       <c r="J10" s="16">
         <f t="shared" si="0"/>
-        <v>1155.4803748523814</v>
+        <v>1884.4630953555445</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
@@ -8217,17 +8217,17 @@
         <v>38</v>
       </c>
       <c r="G11" s="9">
-        <v>-591.46600000000001</v>
+        <v>-1104.06</v>
       </c>
       <c r="H11" s="9">
-        <v>2838.1260000000002</v>
+        <v>2116.1149999999998</v>
       </c>
       <c r="I11" s="9">
-        <v>906.66</v>
+        <v>871.93100000000004</v>
       </c>
       <c r="J11" s="16">
         <f t="shared" si="0"/>
-        <v>3037.5686949651031</v>
+        <v>2541.0932382708825</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
@@ -8248,17 +8248,17 @@
         <v>40</v>
       </c>
       <c r="G12" s="9">
-        <v>-98.260999999999996</v>
+        <v>-149.577</v>
       </c>
       <c r="H12" s="9">
-        <v>655.07299999999998</v>
+        <v>467.428</v>
       </c>
       <c r="I12" s="9">
-        <v>4.9130000000000003</v>
+        <v>3.7389999999999999</v>
       </c>
       <c r="J12" s="16">
         <f t="shared" si="0"/>
-        <v>662.41980421708399</v>
+        <v>490.79139584348866</v>
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
@@ -8279,17 +8279,17 @@
         <v>42</v>
       </c>
       <c r="G13" s="9">
-        <v>98.156999999999996</v>
+        <v>148.98599999999999</v>
       </c>
       <c r="H13" s="9">
-        <v>218.12700000000001</v>
+        <v>310.38799999999998</v>
       </c>
       <c r="I13" s="9">
-        <v>1.6359999999999999</v>
+        <v>2.4830000000000001</v>
       </c>
       <c r="J13" s="16">
         <f t="shared" si="0"/>
-        <v>239.20046252881704</v>
+        <v>344.30176303498649</v>
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
@@ -8310,17 +8310,17 @@
         <v>20</v>
       </c>
       <c r="G14" s="9">
-        <v>4.5999999999999999E-2</v>
+        <v>-5.6000000000000001E-2</v>
       </c>
       <c r="H14" s="9">
-        <v>0.29099999999999998</v>
+        <v>-0.185</v>
       </c>
       <c r="I14" s="9">
-        <v>2.5000000000000001E-2</v>
+        <v>-1.6E-2</v>
       </c>
       <c r="J14" s="16">
         <f t="shared" si="0"/>
-        <v>0.29567211569574831</v>
+        <v>0.19395102474593939</v>
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
@@ -8341,17 +8341,17 @@
         <v>49</v>
       </c>
       <c r="G15" s="9">
-        <v>4.5999999999999999E-2</v>
+        <v>-5.6000000000000001E-2</v>
       </c>
       <c r="H15" s="9">
-        <v>0.29099999999999998</v>
+        <v>-0.185</v>
       </c>
       <c r="I15" s="9">
-        <v>2.5000000000000001E-2</v>
+        <v>-1.6E-2</v>
       </c>
       <c r="J15" s="16">
         <f t="shared" si="0"/>
-        <v>0.29567211569574831</v>
+        <v>0.19395102474593939</v>
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
@@ -8372,17 +8372,17 @@
         <v>53</v>
       </c>
       <c r="G16" s="9">
-        <v>0.28599999999999998</v>
+        <v>0</v>
       </c>
       <c r="H16" s="9">
-        <v>-4657.2939999999999</v>
+        <v>-4305.5630000000001</v>
       </c>
       <c r="I16" s="9">
-        <v>1595.982</v>
+        <v>1352.155</v>
       </c>
       <c r="J16" s="16">
         <f t="shared" si="0"/>
-        <v>4923.1642292895331</v>
+        <v>4512.8921869455289</v>
       </c>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.25">
@@ -8403,17 +8403,17 @@
         <v>57</v>
       </c>
       <c r="G17" s="9">
-        <v>0.28599999999999998</v>
+        <v>0</v>
       </c>
       <c r="H17" s="9">
-        <v>-4657.2939999999999</v>
+        <v>-4305.5630000000001</v>
       </c>
       <c r="I17" s="9">
-        <v>1595.982</v>
+        <v>1352.155</v>
       </c>
       <c r="J17" s="16">
         <f t="shared" si="0"/>
-        <v>4923.1642292895331</v>
+        <v>4512.8921869455289</v>
       </c>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.25">
@@ -8437,14 +8437,14 @@
         <v>0</v>
       </c>
       <c r="H18" s="9">
-        <v>-3373.4340000000002</v>
+        <v>-3332.9589999999998</v>
       </c>
       <c r="I18" s="9">
-        <v>-901.47299999999996</v>
+        <v>-1037.4079999999999</v>
       </c>
       <c r="J18" s="16">
         <f t="shared" si="0"/>
-        <v>3491.8061976697677</v>
+        <v>3490.6777356474768</v>
       </c>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.25">
@@ -8468,14 +8468,14 @@
         <v>0</v>
       </c>
       <c r="H19" s="9">
-        <v>-3373.4340000000002</v>
+        <v>-3332.9589999999998</v>
       </c>
       <c r="I19" s="9">
-        <v>-901.47299999999996</v>
+        <v>-1037.4079999999999</v>
       </c>
       <c r="J19" s="16">
         <f t="shared" si="0"/>
-        <v>3491.8061976697677</v>
+        <v>3490.6777356474768</v>
       </c>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.25">
@@ -8496,17 +8496,17 @@
         <v>20</v>
       </c>
       <c r="G20" s="9">
-        <v>0.28599999999999998</v>
+        <v>0</v>
       </c>
       <c r="H20" s="9">
-        <v>-1283.8599999999999</v>
+        <v>-972.60400000000004</v>
       </c>
       <c r="I20" s="9">
-        <v>2497.4560000000001</v>
+        <v>2389.5619999999999</v>
       </c>
       <c r="J20" s="16">
         <f t="shared" si="0"/>
-        <v>2808.1280336430532</v>
+        <v>2579.9157142550221</v>
       </c>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.25">
@@ -8595,11 +8595,11 @@
         <v>0</v>
       </c>
       <c r="I23" s="9">
-        <v>2288.8910000000001</v>
+        <v>2288.89</v>
       </c>
       <c r="J23" s="16">
         <f t="shared" si="0"/>
-        <v>2288.8910000000001</v>
+        <v>2288.89</v>
       </c>
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.25">
@@ -8626,11 +8626,11 @@
         <v>0</v>
       </c>
       <c r="I24" s="9">
-        <v>522.27099999999996</v>
+        <v>522.27200000000005</v>
       </c>
       <c r="J24" s="16">
         <f t="shared" si="0"/>
-        <v>522.27099999999996</v>
+        <v>522.27200000000005</v>
       </c>
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.25">
@@ -8684,17 +8684,17 @@
         <v>20</v>
       </c>
       <c r="G26" s="9">
-        <v>-914.51700000000005</v>
+        <v>-862.90099999999995</v>
       </c>
       <c r="H26" s="9">
-        <v>-2349.105</v>
+        <v>-2044.0039999999999</v>
       </c>
       <c r="I26" s="9">
-        <v>126.324</v>
+        <v>113.249</v>
       </c>
       <c r="J26" s="16">
         <f t="shared" si="0"/>
-        <v>2524.0034463704683</v>
+        <v>2221.5705759255097</v>
       </c>
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.25">
@@ -8715,17 +8715,17 @@
         <v>20</v>
       </c>
       <c r="G27" s="9">
-        <v>826.42499999999995</v>
+        <v>774.31500000000005</v>
       </c>
       <c r="H27" s="9">
-        <v>-2121.4659999999999</v>
+        <v>-1771.066</v>
       </c>
       <c r="I27" s="9">
-        <v>114.083</v>
+        <v>101.55800000000001</v>
       </c>
       <c r="J27" s="16">
         <f t="shared" si="0"/>
-        <v>2279.6076856928694</v>
+        <v>1935.6013336803114</v>
       </c>
     </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.25">
@@ -8746,17 +8746,17 @@
         <v>20</v>
       </c>
       <c r="G28" s="9">
-        <v>-69.448999999999998</v>
+        <v>-106.26900000000001</v>
       </c>
       <c r="H28" s="9">
-        <v>180.04499999999999</v>
+        <v>275.50200000000001</v>
       </c>
       <c r="I28" s="9">
-        <v>-19.899000000000001</v>
+        <v>-30.449000000000002</v>
       </c>
       <c r="J28" s="16">
         <f t="shared" si="0"/>
-        <v>193.99828820636534</v>
+        <v>296.85281532436238</v>
       </c>
     </row>
     <row r="29" spans="1:10" x14ac:dyDescent="0.25">
@@ -8777,17 +8777,17 @@
         <v>20</v>
       </c>
       <c r="G29" s="9">
-        <v>158.292</v>
+        <v>196.18100000000001</v>
       </c>
       <c r="H29" s="9">
-        <v>427.69299999999998</v>
+        <v>530.06399999999996</v>
       </c>
       <c r="I29" s="9">
-        <v>-47.268999999999998</v>
+        <v>-58.582999999999998</v>
       </c>
       <c r="J29" s="16">
         <f t="shared" si="0"/>
-        <v>458.48884160249742</v>
+        <v>568.23128807379135</v>
       </c>
     </row>
     <row r="30" spans="1:10" x14ac:dyDescent="0.25">
@@ -8808,17 +8808,17 @@
         <v>99</v>
       </c>
       <c r="G30" s="9">
-        <v>158.292</v>
+        <v>196.18100000000001</v>
       </c>
       <c r="H30" s="9">
-        <v>427.69299999999998</v>
+        <v>530.06399999999996</v>
       </c>
       <c r="I30" s="9">
-        <v>-47.268999999999998</v>
+        <v>-58.582999999999998</v>
       </c>
       <c r="J30" s="16">
         <f t="shared" si="0"/>
-        <v>458.48884160249742</v>
+        <v>568.23128807379135</v>
       </c>
     </row>
     <row r="31" spans="1:10" x14ac:dyDescent="0.25">
@@ -8839,17 +8839,17 @@
         <v>101</v>
       </c>
       <c r="G31" s="9">
-        <v>-69.448999999999998</v>
+        <v>-106.26900000000001</v>
       </c>
       <c r="H31" s="9">
-        <v>180.04499999999999</v>
+        <v>275.50200000000001</v>
       </c>
       <c r="I31" s="9">
-        <v>-19.899000000000001</v>
+        <v>-30.449000000000002</v>
       </c>
       <c r="J31" s="16">
         <f t="shared" si="0"/>
-        <v>193.99828820636534</v>
+        <v>296.85281532436238</v>
       </c>
     </row>
     <row r="32" spans="1:10" x14ac:dyDescent="0.25">
@@ -8870,17 +8870,17 @@
         <v>103</v>
       </c>
       <c r="G32" s="9">
-        <v>826.42499999999995</v>
+        <v>774.31500000000005</v>
       </c>
       <c r="H32" s="9">
-        <v>-2121.4659999999999</v>
+        <v>-1771.066</v>
       </c>
       <c r="I32" s="9">
-        <v>114.083</v>
+        <v>101.55800000000001</v>
       </c>
       <c r="J32" s="16">
         <f t="shared" si="0"/>
-        <v>2279.6076856928694</v>
+        <v>1935.6013336803114</v>
       </c>
     </row>
     <row r="33" spans="1:10" x14ac:dyDescent="0.25">
@@ -8901,17 +8901,17 @@
         <v>105</v>
       </c>
       <c r="G33" s="9">
-        <v>-914.51700000000005</v>
+        <v>-862.90099999999995</v>
       </c>
       <c r="H33" s="9">
-        <v>-2349.105</v>
+        <v>-2044.0039999999999</v>
       </c>
       <c r="I33" s="9">
-        <v>126.324</v>
+        <v>113.249</v>
       </c>
       <c r="J33" s="16">
         <f t="shared" si="0"/>
-        <v>2524.0034463704683</v>
+        <v>2221.5705759255097</v>
       </c>
     </row>
     <row r="34" spans="1:10" x14ac:dyDescent="0.25">
@@ -8935,14 +8935,14 @@
         <v>0</v>
       </c>
       <c r="H34" s="9">
-        <v>3789.8609999999999</v>
+        <v>2880.7939999999999</v>
       </c>
       <c r="I34" s="9">
-        <v>2712.692</v>
+        <v>2765.6990000000001</v>
       </c>
       <c r="J34" s="16">
         <f t="shared" si="0"/>
-        <v>4660.6592115477615</v>
+        <v>3993.5028520131295</v>
       </c>
     </row>
     <row r="35" spans="1:10" x14ac:dyDescent="0.25">
@@ -8966,14 +8966,14 @@
         <v>0</v>
       </c>
       <c r="H35" s="9">
-        <v>3789.8609999999999</v>
+        <v>2880.7939999999999</v>
       </c>
       <c r="I35" s="9">
-        <v>2712.692</v>
+        <v>2765.6990000000001</v>
       </c>
       <c r="J35" s="16">
         <f t="shared" si="0"/>
-        <v>4660.6592115477615</v>
+        <v>3993.5028520131295</v>
       </c>
     </row>
     <row r="36" spans="1:10" x14ac:dyDescent="0.25">
@@ -8997,14 +8997,14 @@
         <v>0</v>
       </c>
       <c r="H36" s="9">
-        <v>-315.911</v>
+        <v>-421.73500000000001</v>
       </c>
       <c r="I36" s="9">
-        <v>3094.3519999999999</v>
+        <v>3358.085</v>
       </c>
       <c r="J36" s="16">
         <f t="shared" si="0"/>
-        <v>3110.4363134172991</v>
+        <v>3384.4638094460402</v>
       </c>
     </row>
     <row r="37" spans="1:10" x14ac:dyDescent="0.25">
@@ -9028,14 +9028,14 @@
         <v>0</v>
       </c>
       <c r="H37" s="9">
-        <v>-315.911</v>
+        <v>-421.73500000000001</v>
       </c>
       <c r="I37" s="9">
-        <v>3094.3519999999999</v>
+        <v>3358.085</v>
       </c>
       <c r="J37" s="16">
         <f t="shared" si="0"/>
-        <v>3110.4363134172991</v>
+        <v>3384.4638094460402</v>
       </c>
     </row>
     <row r="38" spans="1:10" x14ac:dyDescent="0.25">
@@ -9056,17 +9056,17 @@
         <v>119</v>
       </c>
       <c r="G38" s="9">
-        <v>-0.752</v>
+        <v>-1.3260000000000001</v>
       </c>
       <c r="H38" s="9">
-        <v>72.971000000000004</v>
+        <v>128.71100000000001</v>
       </c>
       <c r="I38" s="9">
-        <v>-7.2560000000000002</v>
+        <v>-12.798</v>
       </c>
       <c r="J38" s="16">
         <f t="shared" si="0"/>
-        <v>73.334724933008374</v>
+        <v>129.35249746719234</v>
       </c>
     </row>
     <row r="39" spans="1:10" x14ac:dyDescent="0.25">
@@ -9087,17 +9087,17 @@
         <v>20</v>
       </c>
       <c r="G39" s="9">
-        <v>-0.752</v>
+        <v>-1.3260000000000001</v>
       </c>
       <c r="H39" s="9">
-        <v>72.971000000000004</v>
+        <v>128.71100000000001</v>
       </c>
       <c r="I39" s="9">
-        <v>-7.2560000000000002</v>
+        <v>-12.798</v>
       </c>
       <c r="J39" s="16">
         <f t="shared" si="0"/>
-        <v>73.334724933008374</v>
+        <v>129.35249746719234</v>
       </c>
     </row>
     <row r="40" spans="1:10" x14ac:dyDescent="0.25">
@@ -9217,11 +9217,11 @@
         <v>-23.19</v>
       </c>
       <c r="I43" s="9">
-        <v>496.589</v>
+        <v>496.59</v>
       </c>
       <c r="J43" s="16">
         <f t="shared" si="0"/>
-        <v>497.13017520766124</v>
+        <v>497.13117411906484</v>
       </c>
     </row>
     <row r="44" spans="1:10" x14ac:dyDescent="0.25">
@@ -9248,11 +9248,11 @@
         <v>-110.90600000000001</v>
       </c>
       <c r="I44" s="9">
-        <v>2374.922</v>
+        <v>2374.9209999999998</v>
       </c>
       <c r="J44" s="16">
         <f t="shared" si="0"/>
-        <v>2377.5101780930399</v>
+        <v>2377.509179181649</v>
       </c>
     </row>
     <row r="45" spans="1:10" x14ac:dyDescent="0.25">
@@ -9338,14 +9338,14 @@
         <v>0</v>
       </c>
       <c r="H47" s="9">
-        <v>4105.7719999999999</v>
+        <v>3302.529</v>
       </c>
       <c r="I47" s="9">
-        <v>-381.65899999999999</v>
+        <v>-592.38599999999997</v>
       </c>
       <c r="J47" s="16">
         <f t="shared" si="0"/>
-        <v>4123.472724326547</v>
+        <v>3355.2375428331447</v>
       </c>
     </row>
     <row r="48" spans="1:10" x14ac:dyDescent="0.25">
@@ -23912,7 +23912,7 @@
   </sheetPr>
   <dimension ref="A1:J1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B34" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+    <sheetView topLeftCell="B1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <selection activeCell="H48" sqref="H48"/>
     </sheetView>
   </sheetViews>
@@ -33505,7 +33505,7 @@
   <dimension ref="A1:J997"/>
   <sheetViews>
     <sheetView topLeftCell="C1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="M22" sqref="M22"/>
+      <selection activeCell="G3" sqref="G3:I44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>

</xml_diff>